<commit_message>
update with Politi ballot
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="66">
   <si>
     <t>Roy Halladay</t>
   </si>
@@ -212,6 +212,12 @@
   </si>
   <si>
     <t>Barry Bloom</t>
+  </si>
+  <si>
+    <t>Steve Politi</t>
+  </si>
+  <si>
+    <t>NJ.com</t>
   </si>
 </sst>
 </file>
@@ -617,10 +623,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AM15"/>
+  <dimension ref="A1:AM16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1295,6 +1301,50 @@
       </c>
       <c r="AM15" s="1">
         <v>43437</v>
+      </c>
+    </row>
+    <row r="16" spans="1:39">
+      <c r="A16" t="s">
+        <v>64</v>
+      </c>
+      <c r="C16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" t="s">
+        <v>37</v>
+      </c>
+      <c r="I16" t="s">
+        <v>37</v>
+      </c>
+      <c r="K16" t="s">
+        <v>37</v>
+      </c>
+      <c r="M16" t="s">
+        <v>37</v>
+      </c>
+      <c r="N16" t="s">
+        <v>37</v>
+      </c>
+      <c r="O16" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>37</v>
+      </c>
+      <c r="V16" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK16">
+        <v>10</v>
+      </c>
+      <c r="AL16" t="s">
+        <v>65</v>
+      </c>
+      <c r="AM16" s="1">
+        <v>43439</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add Dunn and Herzog ballots
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="69">
   <si>
     <t>Roy Halladay</t>
   </si>
@@ -218,6 +218,15 @@
   </si>
   <si>
     <t>NJ.com</t>
+  </si>
+  <si>
+    <t>Jay Dunn</t>
+  </si>
+  <si>
+    <t>The Trentonian</t>
+  </si>
+  <si>
+    <t>Bob Herzog</t>
   </si>
 </sst>
 </file>
@@ -623,10 +632,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AM16"/>
+  <dimension ref="A1:AM18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="AB1" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1344,6 +1353,88 @@
         <v>65</v>
       </c>
       <c r="AM16" s="1">
+        <v>43439</v>
+      </c>
+    </row>
+    <row r="17" spans="1:39">
+      <c r="A17" t="s">
+        <v>66</v>
+      </c>
+      <c r="E17" t="s">
+        <v>37</v>
+      </c>
+      <c r="I17" t="s">
+        <v>37</v>
+      </c>
+      <c r="J17" t="s">
+        <v>37</v>
+      </c>
+      <c r="K17" t="s">
+        <v>37</v>
+      </c>
+      <c r="M17" t="s">
+        <v>37</v>
+      </c>
+      <c r="O17" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>37</v>
+      </c>
+      <c r="T17" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK17">
+        <v>8</v>
+      </c>
+      <c r="AL17" t="s">
+        <v>67</v>
+      </c>
+      <c r="AM17" s="1">
+        <v>43439</v>
+      </c>
+    </row>
+    <row r="18" spans="1:39">
+      <c r="A18" t="s">
+        <v>68</v>
+      </c>
+      <c r="C18" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" t="s">
+        <v>37</v>
+      </c>
+      <c r="E18" t="s">
+        <v>37</v>
+      </c>
+      <c r="F18" t="s">
+        <v>37</v>
+      </c>
+      <c r="H18" t="s">
+        <v>37</v>
+      </c>
+      <c r="I18" t="s">
+        <v>37</v>
+      </c>
+      <c r="J18" t="s">
+        <v>37</v>
+      </c>
+      <c r="K18" t="s">
+        <v>37</v>
+      </c>
+      <c r="O18" t="s">
+        <v>37</v>
+      </c>
+      <c r="V18" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK18">
+        <v>10</v>
+      </c>
+      <c r="AL18" t="s">
+        <v>44</v>
+      </c>
+      <c r="AM18" s="1">
         <v>43439</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update with Bill Center ballot
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="71">
   <si>
     <t>Roy Halladay</t>
   </si>
@@ -227,6 +227,12 @@
   </si>
   <si>
     <t>Bob Herzog</t>
+  </si>
+  <si>
+    <t>Bill Center</t>
+  </si>
+  <si>
+    <t>DM</t>
   </si>
 </sst>
 </file>
@@ -632,10 +638,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AM18"/>
+  <dimension ref="A1:AM19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AB1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1435,6 +1441,50 @@
         <v>44</v>
       </c>
       <c r="AM18" s="1">
+        <v>43439</v>
+      </c>
+    </row>
+    <row r="19" spans="1:39">
+      <c r="A19" t="s">
+        <v>69</v>
+      </c>
+      <c r="C19" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" t="s">
+        <v>37</v>
+      </c>
+      <c r="E19" t="s">
+        <v>37</v>
+      </c>
+      <c r="F19" t="s">
+        <v>37</v>
+      </c>
+      <c r="I19" t="s">
+        <v>37</v>
+      </c>
+      <c r="J19" t="s">
+        <v>37</v>
+      </c>
+      <c r="K19" t="s">
+        <v>37</v>
+      </c>
+      <c r="O19" t="s">
+        <v>37</v>
+      </c>
+      <c r="T19" t="s">
+        <v>37</v>
+      </c>
+      <c r="V19" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK19">
+        <v>10</v>
+      </c>
+      <c r="AL19" t="s">
+        <v>70</v>
+      </c>
+      <c r="AM19" s="1">
         <v>43439</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update with Jon Heyman ballot
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="73">
   <si>
     <t>Roy Halladay</t>
   </si>
@@ -233,6 +233,12 @@
   </si>
   <si>
     <t>DM</t>
+  </si>
+  <si>
+    <t>Jon Heyman</t>
+  </si>
+  <si>
+    <t>Fancred</t>
   </si>
 </sst>
 </file>
@@ -638,10 +644,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AM19"/>
+  <dimension ref="A1:AM20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1486,6 +1492,50 @@
       </c>
       <c r="AM19" s="1">
         <v>43439</v>
+      </c>
+    </row>
+    <row r="20" spans="1:39">
+      <c r="A20" t="s">
+        <v>71</v>
+      </c>
+      <c r="B20" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" t="s">
+        <v>37</v>
+      </c>
+      <c r="E20" t="s">
+        <v>37</v>
+      </c>
+      <c r="G20" t="s">
+        <v>37</v>
+      </c>
+      <c r="I20" t="s">
+        <v>37</v>
+      </c>
+      <c r="J20" t="s">
+        <v>37</v>
+      </c>
+      <c r="K20" t="s">
+        <v>37</v>
+      </c>
+      <c r="O20" t="s">
+        <v>37</v>
+      </c>
+      <c r="P20" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK20">
+        <v>10</v>
+      </c>
+      <c r="AL20" t="s">
+        <v>72</v>
+      </c>
+      <c r="AM20" s="1">
+        <v>43440</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update with D'Angelo and Plunkett ballots
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="75">
   <si>
     <t>Roy Halladay</t>
   </si>
@@ -239,6 +239,12 @@
   </si>
   <si>
     <t>Fancred</t>
+  </si>
+  <si>
+    <t>Tom D'Angelo</t>
+  </si>
+  <si>
+    <t>Bill Plunkett</t>
   </si>
 </sst>
 </file>
@@ -644,10 +650,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AM20"/>
+  <dimension ref="A1:AM22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1536,6 +1542,82 @@
       </c>
       <c r="AM20" s="1">
         <v>43440</v>
+      </c>
+    </row>
+    <row r="21" spans="1:39">
+      <c r="A21" t="s">
+        <v>73</v>
+      </c>
+      <c r="C21" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21" t="s">
+        <v>37</v>
+      </c>
+      <c r="E21" t="s">
+        <v>37</v>
+      </c>
+      <c r="I21" t="s">
+        <v>37</v>
+      </c>
+      <c r="K21" t="s">
+        <v>37</v>
+      </c>
+      <c r="N21" t="s">
+        <v>37</v>
+      </c>
+      <c r="O21" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>37</v>
+      </c>
+      <c r="T21" t="s">
+        <v>37</v>
+      </c>
+      <c r="V21" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK21">
+        <v>10</v>
+      </c>
+      <c r="AL21" t="s">
+        <v>70</v>
+      </c>
+      <c r="AM21" s="1">
+        <v>43441</v>
+      </c>
+    </row>
+    <row r="22" spans="1:39">
+      <c r="A22" t="s">
+        <v>74</v>
+      </c>
+      <c r="E22" t="s">
+        <v>37</v>
+      </c>
+      <c r="F22" t="s">
+        <v>37</v>
+      </c>
+      <c r="I22" t="s">
+        <v>37</v>
+      </c>
+      <c r="O22" t="s">
+        <v>37</v>
+      </c>
+      <c r="R22" t="s">
+        <v>37</v>
+      </c>
+      <c r="V22" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK22">
+        <v>6</v>
+      </c>
+      <c r="AL22" t="s">
+        <v>38</v>
+      </c>
+      <c r="AM22" s="1">
+        <v>43441</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update with Dubow ballot
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="76">
   <si>
     <t>Roy Halladay</t>
   </si>
@@ -245,6 +245,9 @@
   </si>
   <si>
     <t>Bill Plunkett</t>
+  </si>
+  <si>
+    <t>Josh Dubow</t>
   </si>
 </sst>
 </file>
@@ -650,10 +653,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AM22"/>
+  <dimension ref="A1:AM23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1617,6 +1620,50 @@
         <v>38</v>
       </c>
       <c r="AM22" s="1">
+        <v>43441</v>
+      </c>
+    </row>
+    <row r="23" spans="1:39">
+      <c r="A23" t="s">
+        <v>75</v>
+      </c>
+      <c r="C23" t="s">
+        <v>37</v>
+      </c>
+      <c r="D23" t="s">
+        <v>37</v>
+      </c>
+      <c r="E23" t="s">
+        <v>37</v>
+      </c>
+      <c r="I23" t="s">
+        <v>37</v>
+      </c>
+      <c r="K23" t="s">
+        <v>37</v>
+      </c>
+      <c r="N23" t="s">
+        <v>37</v>
+      </c>
+      <c r="O23" t="s">
+        <v>37</v>
+      </c>
+      <c r="P23" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>37</v>
+      </c>
+      <c r="V23" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK23">
+        <v>10</v>
+      </c>
+      <c r="AL23" t="s">
+        <v>44</v>
+      </c>
+      <c r="AM23" s="1">
         <v>43441</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update with Cardenas ballot
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="77">
   <si>
     <t>Roy Halladay</t>
   </si>
@@ -248,6 +248,9 @@
   </si>
   <si>
     <t>Josh Dubow</t>
+  </si>
+  <si>
+    <t>René Cárdenas</t>
   </si>
 </sst>
 </file>
@@ -653,10 +656,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AM23"/>
+  <dimension ref="A1:AM24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1664,6 +1667,50 @@
         <v>44</v>
       </c>
       <c r="AM23" s="1">
+        <v>43441</v>
+      </c>
+    </row>
+    <row r="24" spans="1:39">
+      <c r="A24" t="s">
+        <v>76</v>
+      </c>
+      <c r="B24" t="s">
+        <v>37</v>
+      </c>
+      <c r="D24" t="s">
+        <v>37</v>
+      </c>
+      <c r="H24" t="s">
+        <v>37</v>
+      </c>
+      <c r="I24" t="s">
+        <v>37</v>
+      </c>
+      <c r="L24" t="s">
+        <v>37</v>
+      </c>
+      <c r="O24" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>37</v>
+      </c>
+      <c r="T24" t="s">
+        <v>37</v>
+      </c>
+      <c r="U24" t="s">
+        <v>37</v>
+      </c>
+      <c r="V24" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK24">
+        <v>10</v>
+      </c>
+      <c r="AL24" t="s">
+        <v>44</v>
+      </c>
+      <c r="AM24" s="1">
         <v>43441</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add Tim Booth ballot
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="78">
   <si>
     <t>Roy Halladay</t>
   </si>
@@ -251,6 +251,9 @@
   </si>
   <si>
     <t>René Cárdenas</t>
+  </si>
+  <si>
+    <t>Tim Booth</t>
   </si>
 </sst>
 </file>
@@ -656,10 +659,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AM24"/>
+  <dimension ref="A1:AM25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1711,6 +1714,50 @@
         <v>44</v>
       </c>
       <c r="AM24" s="1">
+        <v>43441</v>
+      </c>
+    </row>
+    <row r="25" spans="1:39">
+      <c r="A25" t="s">
+        <v>77</v>
+      </c>
+      <c r="C25" t="s">
+        <v>37</v>
+      </c>
+      <c r="D25" t="s">
+        <v>37</v>
+      </c>
+      <c r="E25" t="s">
+        <v>37</v>
+      </c>
+      <c r="F25" t="s">
+        <v>37</v>
+      </c>
+      <c r="I25" t="s">
+        <v>37</v>
+      </c>
+      <c r="K25" t="s">
+        <v>37</v>
+      </c>
+      <c r="O25" t="s">
+        <v>37</v>
+      </c>
+      <c r="P25" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>37</v>
+      </c>
+      <c r="V25" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK25">
+        <v>10</v>
+      </c>
+      <c r="AL25" t="s">
+        <v>44</v>
+      </c>
+      <c r="AM25" s="1">
         <v>43441</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add Simmons, Stewart, Newhan, and Rangel ballots
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="83">
   <si>
     <t>Roy Halladay</t>
   </si>
@@ -254,6 +254,21 @@
   </si>
   <si>
     <t>Tim Booth</t>
+  </si>
+  <si>
+    <t>Steve Simmons</t>
+  </si>
+  <si>
+    <t>Toronto Sun</t>
+  </si>
+  <si>
+    <t>Carl Steward</t>
+  </si>
+  <si>
+    <t>Ross Newhan</t>
+  </si>
+  <si>
+    <t>Luis Rangel</t>
   </si>
 </sst>
 </file>
@@ -659,10 +674,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AM25"/>
+  <dimension ref="A1:AM29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1759,6 +1774,173 @@
       </c>
       <c r="AM25" s="1">
         <v>43441</v>
+      </c>
+    </row>
+    <row r="26" spans="1:39">
+      <c r="A26" t="s">
+        <v>78</v>
+      </c>
+      <c r="E26" t="s">
+        <v>37</v>
+      </c>
+      <c r="I26" t="s">
+        <v>37</v>
+      </c>
+      <c r="J26" t="s">
+        <v>37</v>
+      </c>
+      <c r="K26" t="s">
+        <v>37</v>
+      </c>
+      <c r="O26" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>37</v>
+      </c>
+      <c r="T26" t="s">
+        <v>37</v>
+      </c>
+      <c r="V26" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK26">
+        <v>8</v>
+      </c>
+      <c r="AL26" t="s">
+        <v>79</v>
+      </c>
+      <c r="AM26" s="1">
+        <v>43442</v>
+      </c>
+    </row>
+    <row r="27" spans="1:39">
+      <c r="A27" t="s">
+        <v>80</v>
+      </c>
+      <c r="C27" t="s">
+        <v>37</v>
+      </c>
+      <c r="D27" t="s">
+        <v>37</v>
+      </c>
+      <c r="E27" t="s">
+        <v>37</v>
+      </c>
+      <c r="H27" t="s">
+        <v>37</v>
+      </c>
+      <c r="I27" t="s">
+        <v>37</v>
+      </c>
+      <c r="K27" t="s">
+        <v>37</v>
+      </c>
+      <c r="O27" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>37</v>
+      </c>
+      <c r="T27" t="s">
+        <v>37</v>
+      </c>
+      <c r="V27" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK27">
+        <v>10</v>
+      </c>
+      <c r="AL27" t="s">
+        <v>44</v>
+      </c>
+      <c r="AM27" s="1">
+        <v>43442</v>
+      </c>
+    </row>
+    <row r="28" spans="1:39">
+      <c r="A28" t="s">
+        <v>81</v>
+      </c>
+      <c r="E28" t="s">
+        <v>37</v>
+      </c>
+      <c r="H28" t="s">
+        <v>37</v>
+      </c>
+      <c r="I28" t="s">
+        <v>37</v>
+      </c>
+      <c r="J28" t="s">
+        <v>37</v>
+      </c>
+      <c r="K28" t="s">
+        <v>37</v>
+      </c>
+      <c r="O28" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>37</v>
+      </c>
+      <c r="T28" t="s">
+        <v>37</v>
+      </c>
+      <c r="V28" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK28">
+        <v>9</v>
+      </c>
+      <c r="AL28" t="s">
+        <v>44</v>
+      </c>
+      <c r="AM28" s="1">
+        <v>43442</v>
+      </c>
+    </row>
+    <row r="29" spans="1:39">
+      <c r="A29" t="s">
+        <v>82</v>
+      </c>
+      <c r="C29" t="s">
+        <v>37</v>
+      </c>
+      <c r="D29" t="s">
+        <v>37</v>
+      </c>
+      <c r="E29" t="s">
+        <v>37</v>
+      </c>
+      <c r="I29" t="s">
+        <v>37</v>
+      </c>
+      <c r="K29" t="s">
+        <v>37</v>
+      </c>
+      <c r="N29" t="s">
+        <v>37</v>
+      </c>
+      <c r="O29" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>37</v>
+      </c>
+      <c r="R29" t="s">
+        <v>37</v>
+      </c>
+      <c r="S29" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK29">
+        <v>10</v>
+      </c>
+      <c r="AL29" t="s">
+        <v>44</v>
+      </c>
+      <c r="AM29" s="1">
+        <v>43443</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update with Gaddis ballot
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="84">
   <si>
     <t>Roy Halladay</t>
   </si>
@@ -269,6 +269,9 @@
   </si>
   <si>
     <t>Luis Rangel</t>
+  </si>
+  <si>
+    <t>Carter Gaddis</t>
   </si>
 </sst>
 </file>
@@ -674,10 +677,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AM29"/>
+  <dimension ref="A1:AM30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1940,6 +1946,44 @@
         <v>44</v>
       </c>
       <c r="AM29" s="1">
+        <v>43443</v>
+      </c>
+    </row>
+    <row r="30" spans="1:39">
+      <c r="A30" t="s">
+        <v>83</v>
+      </c>
+      <c r="E30" t="s">
+        <v>37</v>
+      </c>
+      <c r="F30" t="s">
+        <v>37</v>
+      </c>
+      <c r="I30" t="s">
+        <v>37</v>
+      </c>
+      <c r="J30" t="s">
+        <v>37</v>
+      </c>
+      <c r="K30" t="s">
+        <v>37</v>
+      </c>
+      <c r="O30" t="s">
+        <v>37</v>
+      </c>
+      <c r="T30" t="s">
+        <v>37</v>
+      </c>
+      <c r="V30" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK30">
+        <v>8</v>
+      </c>
+      <c r="AL30" t="s">
+        <v>70</v>
+      </c>
+      <c r="AM30" s="1">
         <v>43443</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add Stone and White ballots
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="86">
   <si>
     <t>Roy Halladay</t>
   </si>
@@ -272,6 +272,12 @@
   </si>
   <si>
     <t>Carter Gaddis</t>
+  </si>
+  <si>
+    <t>Larry Stone</t>
+  </si>
+  <si>
+    <t>Paul White</t>
   </si>
 </sst>
 </file>
@@ -320,8 +326,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -337,17 +347,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -677,13 +691,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AM30"/>
+  <dimension ref="A1:AM32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B30" sqref="B30"/>
+      <selection pane="bottomRight" activeCell="AM28" sqref="AM28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1985,6 +1999,91 @@
       </c>
       <c r="AM30" s="1">
         <v>43443</v>
+      </c>
+    </row>
+    <row r="31" spans="1:39">
+      <c r="A31" t="s">
+        <v>84</v>
+      </c>
+      <c r="C31" t="s">
+        <v>37</v>
+      </c>
+      <c r="D31" t="s">
+        <v>37</v>
+      </c>
+      <c r="E31" t="s">
+        <v>37</v>
+      </c>
+      <c r="F31" t="s">
+        <v>37</v>
+      </c>
+      <c r="I31" t="s">
+        <v>37</v>
+      </c>
+      <c r="J31" t="s">
+        <v>37</v>
+      </c>
+      <c r="K31" t="s">
+        <v>37</v>
+      </c>
+      <c r="O31" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>37</v>
+      </c>
+      <c r="V31" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK31">
+        <v>10</v>
+      </c>
+      <c r="AL31" t="s">
+        <v>44</v>
+      </c>
+      <c r="AM31" s="1">
+        <v>43444</v>
+      </c>
+    </row>
+    <row r="32" spans="1:39">
+      <c r="A32" t="s">
+        <v>85</v>
+      </c>
+      <c r="E32" t="s">
+        <v>37</v>
+      </c>
+      <c r="F32" t="s">
+        <v>37</v>
+      </c>
+      <c r="I32" t="s">
+        <v>37</v>
+      </c>
+      <c r="K32" t="s">
+        <v>37</v>
+      </c>
+      <c r="O32" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>37</v>
+      </c>
+      <c r="R32" t="s">
+        <v>37</v>
+      </c>
+      <c r="U32" t="s">
+        <v>37</v>
+      </c>
+      <c r="V32" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK32">
+        <v>9</v>
+      </c>
+      <c r="AL32" t="s">
+        <v>38</v>
+      </c>
+      <c r="AM32" s="1">
+        <v>43444</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add Jay Cohen ballot
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="88">
   <si>
     <t>Roy Halladay</t>
   </si>
@@ -278,6 +278,12 @@
   </si>
   <si>
     <t>Paul White</t>
+  </si>
+  <si>
+    <t>Jay Cohen</t>
+  </si>
+  <si>
+    <t>not specified</t>
   </si>
 </sst>
 </file>
@@ -691,13 +697,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AM32"/>
+  <dimension ref="A1:AM33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AH5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AM28" sqref="AM28"/>
+      <selection pane="bottomRight" activeCell="AL33" sqref="AL33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2083,6 +2089,50 @@
         <v>38</v>
       </c>
       <c r="AM32" s="1">
+        <v>43444</v>
+      </c>
+    </row>
+    <row r="33" spans="1:39">
+      <c r="A33" t="s">
+        <v>86</v>
+      </c>
+      <c r="C33" t="s">
+        <v>37</v>
+      </c>
+      <c r="D33" t="s">
+        <v>37</v>
+      </c>
+      <c r="E33" t="s">
+        <v>37</v>
+      </c>
+      <c r="I33" t="s">
+        <v>37</v>
+      </c>
+      <c r="J33" t="s">
+        <v>37</v>
+      </c>
+      <c r="K33" t="s">
+        <v>37</v>
+      </c>
+      <c r="O33" t="s">
+        <v>37</v>
+      </c>
+      <c r="P33" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>37</v>
+      </c>
+      <c r="V33" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK33">
+        <v>10</v>
+      </c>
+      <c r="AL33" t="s">
+        <v>87</v>
+      </c>
+      <c r="AM33" s="1">
         <v>43444</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Graham and McCaffery ballots
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="91">
   <si>
     <t>Roy Halladay</t>
   </si>
@@ -287,6 +287,12 @@
   </si>
   <si>
     <t>David Maril</t>
+  </si>
+  <si>
+    <t>Patrick Graham</t>
+  </si>
+  <si>
+    <t>Jack McCaffery</t>
   </si>
 </sst>
 </file>
@@ -700,13 +706,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AM34"/>
+  <dimension ref="A1:AM36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Y27" sqref="Y27"/>
+      <selection pane="bottomRight" activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2178,6 +2184,94 @@
       </c>
       <c r="AM34" s="1">
         <v>43445</v>
+      </c>
+    </row>
+    <row r="35" spans="1:39">
+      <c r="A35" t="s">
+        <v>89</v>
+      </c>
+      <c r="C35" t="s">
+        <v>37</v>
+      </c>
+      <c r="D35" t="s">
+        <v>37</v>
+      </c>
+      <c r="E35" t="s">
+        <v>37</v>
+      </c>
+      <c r="F35" t="s">
+        <v>37</v>
+      </c>
+      <c r="I35" t="s">
+        <v>37</v>
+      </c>
+      <c r="K35" t="s">
+        <v>37</v>
+      </c>
+      <c r="O35" t="s">
+        <v>37</v>
+      </c>
+      <c r="P35" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>37</v>
+      </c>
+      <c r="V35" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK35">
+        <v>10</v>
+      </c>
+      <c r="AL35" t="s">
+        <v>44</v>
+      </c>
+      <c r="AM35" s="1">
+        <v>43446</v>
+      </c>
+    </row>
+    <row r="36" spans="1:39">
+      <c r="A36" t="s">
+        <v>90</v>
+      </c>
+      <c r="C36" t="s">
+        <v>37</v>
+      </c>
+      <c r="D36" t="s">
+        <v>37</v>
+      </c>
+      <c r="E36" t="s">
+        <v>37</v>
+      </c>
+      <c r="G36" t="s">
+        <v>37</v>
+      </c>
+      <c r="I36" t="s">
+        <v>37</v>
+      </c>
+      <c r="J36" t="s">
+        <v>37</v>
+      </c>
+      <c r="O36" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>37</v>
+      </c>
+      <c r="T36" t="s">
+        <v>37</v>
+      </c>
+      <c r="V36" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK36">
+        <v>10</v>
+      </c>
+      <c r="AL36" t="s">
+        <v>44</v>
+      </c>
+      <c r="AM36" s="1">
+        <v>43446</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Vene and Biertempfel ballots
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="95">
   <si>
     <t>Roy Halladay</t>
   </si>
@@ -293,6 +293,18 @@
   </si>
   <si>
     <t>Jack McCaffery</t>
+  </si>
+  <si>
+    <t>Juan Vené</t>
+  </si>
+  <si>
+    <t>JuanVene.com</t>
+  </si>
+  <si>
+    <t>Rob Biertempfel</t>
+  </si>
+  <si>
+    <t>twitter</t>
   </si>
 </sst>
 </file>
@@ -706,13 +718,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AM36"/>
+  <dimension ref="A1:AM38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B37" sqref="B37"/>
+      <selection pane="bottomRight" activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2272,6 +2284,64 @@
       </c>
       <c r="AM36" s="1">
         <v>43446</v>
+      </c>
+    </row>
+    <row r="37" spans="1:39">
+      <c r="A37" t="s">
+        <v>91</v>
+      </c>
+      <c r="F37" t="s">
+        <v>37</v>
+      </c>
+      <c r="J37" t="s">
+        <v>37</v>
+      </c>
+      <c r="K37" t="s">
+        <v>37</v>
+      </c>
+      <c r="M37" t="s">
+        <v>37</v>
+      </c>
+      <c r="O37" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK37">
+        <v>5</v>
+      </c>
+      <c r="AL37" t="s">
+        <v>92</v>
+      </c>
+      <c r="AM37" s="1">
+        <v>43447</v>
+      </c>
+    </row>
+    <row r="38" spans="1:39">
+      <c r="A38" t="s">
+        <v>93</v>
+      </c>
+      <c r="E38" t="s">
+        <v>37</v>
+      </c>
+      <c r="K38" t="s">
+        <v>37</v>
+      </c>
+      <c r="O38" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>37</v>
+      </c>
+      <c r="V38" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK38">
+        <v>5</v>
+      </c>
+      <c r="AL38" t="s">
+        <v>94</v>
+      </c>
+      <c r="AM38" s="1">
+        <v>43447</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add Lennon and Caputo ballots
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="103">
   <si>
     <t>Roy Halladay</t>
   </si>
@@ -320,6 +320,15 @@
   </si>
   <si>
     <t>unknown</t>
+  </si>
+  <si>
+    <t>David Lennon</t>
+  </si>
+  <si>
+    <t>Pat Caputo</t>
+  </si>
+  <si>
+    <t>Oakland Press</t>
   </si>
 </sst>
 </file>
@@ -735,13 +744,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AM41"/>
+  <dimension ref="A1:AM43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AE13" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AL41" sqref="AL41"/>
+      <selection pane="bottomRight" activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2473,6 +2482,73 @@
       </c>
       <c r="AM41" s="1">
         <v>43447</v>
+      </c>
+    </row>
+    <row r="42" spans="1:39">
+      <c r="A42" t="s">
+        <v>100</v>
+      </c>
+      <c r="C42" t="s">
+        <v>37</v>
+      </c>
+      <c r="D42" t="s">
+        <v>37</v>
+      </c>
+      <c r="O42" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK42">
+        <v>3</v>
+      </c>
+      <c r="AL42" t="s">
+        <v>46</v>
+      </c>
+      <c r="AM42" s="1">
+        <v>43448</v>
+      </c>
+    </row>
+    <row r="43" spans="1:39">
+      <c r="A43" t="s">
+        <v>101</v>
+      </c>
+      <c r="C43" t="s">
+        <v>37</v>
+      </c>
+      <c r="D43" t="s">
+        <v>37</v>
+      </c>
+      <c r="E43" t="s">
+        <v>37</v>
+      </c>
+      <c r="I43" t="s">
+        <v>37</v>
+      </c>
+      <c r="K43" t="s">
+        <v>37</v>
+      </c>
+      <c r="N43" t="s">
+        <v>37</v>
+      </c>
+      <c r="O43" t="s">
+        <v>37</v>
+      </c>
+      <c r="P43" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q43" t="s">
+        <v>37</v>
+      </c>
+      <c r="V43" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK43">
+        <v>10</v>
+      </c>
+      <c r="AL43" t="s">
+        <v>102</v>
+      </c>
+      <c r="AM43" s="1">
+        <v>43448</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add Rubin and Shalin ballots
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="106">
   <si>
     <t>Roy Halladay</t>
   </si>
@@ -329,6 +329,15 @@
   </si>
   <si>
     <t>Oakland Press</t>
+  </si>
+  <si>
+    <t>Roger Rubin</t>
+  </si>
+  <si>
+    <t>Newsday+Twitter</t>
+  </si>
+  <si>
+    <t>Mike Shalin</t>
   </si>
 </sst>
 </file>
@@ -744,13 +753,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AM43"/>
+  <dimension ref="A1:AM45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G37" sqref="G37"/>
+      <selection pane="bottomRight" activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2548,6 +2557,82 @@
         <v>102</v>
       </c>
       <c r="AM43" s="1">
+        <v>43448</v>
+      </c>
+    </row>
+    <row r="44" spans="1:39">
+      <c r="A44" t="s">
+        <v>103</v>
+      </c>
+      <c r="C44" t="s">
+        <v>37</v>
+      </c>
+      <c r="D44" t="s">
+        <v>37</v>
+      </c>
+      <c r="E44" t="s">
+        <v>37</v>
+      </c>
+      <c r="I44" t="s">
+        <v>37</v>
+      </c>
+      <c r="O44" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q44" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK44">
+        <v>6</v>
+      </c>
+      <c r="AL44" t="s">
+        <v>104</v>
+      </c>
+      <c r="AM44" s="1">
+        <v>43448</v>
+      </c>
+    </row>
+    <row r="45" spans="1:39">
+      <c r="A45" t="s">
+        <v>105</v>
+      </c>
+      <c r="C45" t="s">
+        <v>37</v>
+      </c>
+      <c r="D45" t="s">
+        <v>37</v>
+      </c>
+      <c r="E45" t="s">
+        <v>37</v>
+      </c>
+      <c r="H45" t="s">
+        <v>37</v>
+      </c>
+      <c r="I45" t="s">
+        <v>37</v>
+      </c>
+      <c r="K45" t="s">
+        <v>37</v>
+      </c>
+      <c r="O45" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q45" t="s">
+        <v>37</v>
+      </c>
+      <c r="T45" t="s">
+        <v>37</v>
+      </c>
+      <c r="V45" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK45">
+        <v>10</v>
+      </c>
+      <c r="AL45" t="s">
+        <v>44</v>
+      </c>
+      <c r="AM45" s="1">
         <v>43448</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add 5 new ballots from 12/15-12/16
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="110">
   <si>
     <t>Roy Halladay</t>
   </si>
@@ -338,6 +338,18 @@
   </si>
   <si>
     <t>Mike Shalin</t>
+  </si>
+  <si>
+    <t>Mark Newman</t>
+  </si>
+  <si>
+    <t>Richard Justice</t>
+  </si>
+  <si>
+    <t>Mark Hale</t>
+  </si>
+  <si>
+    <t>Jeff Blair</t>
   </si>
 </sst>
 </file>
@@ -753,13 +765,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AM45"/>
+  <dimension ref="A1:AM49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B45" sqref="B45"/>
+      <selection pane="bottomRight" activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2634,6 +2646,164 @@
       </c>
       <c r="AM45" s="1">
         <v>43448</v>
+      </c>
+    </row>
+    <row r="46" spans="1:39">
+      <c r="A46" t="s">
+        <v>106</v>
+      </c>
+      <c r="C46" t="s">
+        <v>37</v>
+      </c>
+      <c r="D46" t="s">
+        <v>37</v>
+      </c>
+      <c r="E46" t="s">
+        <v>37</v>
+      </c>
+      <c r="I46" t="s">
+        <v>37</v>
+      </c>
+      <c r="K46" t="s">
+        <v>37</v>
+      </c>
+      <c r="M46" t="s">
+        <v>37</v>
+      </c>
+      <c r="O46" t="s">
+        <v>37</v>
+      </c>
+      <c r="P46" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q46" t="s">
+        <v>37</v>
+      </c>
+      <c r="V46" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK46">
+        <v>10</v>
+      </c>
+      <c r="AL46" t="s">
+        <v>44</v>
+      </c>
+      <c r="AM46" s="1">
+        <v>43450</v>
+      </c>
+    </row>
+    <row r="47" spans="1:39">
+      <c r="A47" t="s">
+        <v>107</v>
+      </c>
+      <c r="C47" t="s">
+        <v>37</v>
+      </c>
+      <c r="D47" t="s">
+        <v>37</v>
+      </c>
+      <c r="E47" t="s">
+        <v>37</v>
+      </c>
+      <c r="I47" t="s">
+        <v>37</v>
+      </c>
+      <c r="K47" t="s">
+        <v>37</v>
+      </c>
+      <c r="O47" t="s">
+        <v>37</v>
+      </c>
+      <c r="P47" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q47" t="s">
+        <v>37</v>
+      </c>
+      <c r="U47" t="s">
+        <v>37</v>
+      </c>
+      <c r="V47" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK47">
+        <v>10</v>
+      </c>
+      <c r="AL47" t="s">
+        <v>38</v>
+      </c>
+      <c r="AM47" s="1">
+        <v>43449</v>
+      </c>
+    </row>
+    <row r="48" spans="1:39">
+      <c r="A48" t="s">
+        <v>108</v>
+      </c>
+      <c r="C48" t="s">
+        <v>37</v>
+      </c>
+      <c r="D48" t="s">
+        <v>37</v>
+      </c>
+      <c r="E48" t="s">
+        <v>37</v>
+      </c>
+      <c r="I48" t="s">
+        <v>37</v>
+      </c>
+      <c r="K48" t="s">
+        <v>37</v>
+      </c>
+      <c r="N48" t="s">
+        <v>37</v>
+      </c>
+      <c r="O48" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q48" t="s">
+        <v>37</v>
+      </c>
+      <c r="V48" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK48">
+        <v>9</v>
+      </c>
+      <c r="AL48" t="s">
+        <v>44</v>
+      </c>
+      <c r="AM48" s="1">
+        <v>43449</v>
+      </c>
+    </row>
+    <row r="49" spans="1:39">
+      <c r="A49" t="s">
+        <v>109</v>
+      </c>
+      <c r="C49" t="s">
+        <v>37</v>
+      </c>
+      <c r="D49" t="s">
+        <v>37</v>
+      </c>
+      <c r="E49" t="s">
+        <v>37</v>
+      </c>
+      <c r="O49" t="s">
+        <v>37</v>
+      </c>
+      <c r="V49" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK49">
+        <v>5</v>
+      </c>
+      <c r="AL49" t="s">
+        <v>44</v>
+      </c>
+      <c r="AM49" s="1">
+        <v>43449</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update with 12/17 ballots
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="115">
   <si>
     <t>Roy Halladay</t>
   </si>
@@ -350,6 +350,21 @@
   </si>
   <si>
     <t>Jeff Blair</t>
+  </si>
+  <si>
+    <t>Roberto Colon</t>
+  </si>
+  <si>
+    <t>Unanimo Sports</t>
+  </si>
+  <si>
+    <t>Greg Cote</t>
+  </si>
+  <si>
+    <t>Felix DeJesus</t>
+  </si>
+  <si>
+    <t>Mike Vaccaro</t>
   </si>
 </sst>
 </file>
@@ -765,13 +780,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AM49"/>
+  <dimension ref="A1:AM53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B49" sqref="B49"/>
+      <selection pane="bottomRight" activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2804,6 +2819,179 @@
       </c>
       <c r="AM49" s="1">
         <v>43449</v>
+      </c>
+    </row>
+    <row r="50" spans="1:39">
+      <c r="A50" t="s">
+        <v>110</v>
+      </c>
+      <c r="C50" t="s">
+        <v>37</v>
+      </c>
+      <c r="D50" t="s">
+        <v>37</v>
+      </c>
+      <c r="E50" t="s">
+        <v>37</v>
+      </c>
+      <c r="I50" t="s">
+        <v>37</v>
+      </c>
+      <c r="J50" t="s">
+        <v>37</v>
+      </c>
+      <c r="K50" t="s">
+        <v>37</v>
+      </c>
+      <c r="O50" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q50" t="s">
+        <v>37</v>
+      </c>
+      <c r="S50" t="s">
+        <v>37</v>
+      </c>
+      <c r="T50" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK50">
+        <v>10</v>
+      </c>
+      <c r="AL50" t="s">
+        <v>111</v>
+      </c>
+      <c r="AM50" s="1">
+        <v>43451</v>
+      </c>
+    </row>
+    <row r="51" spans="1:39">
+      <c r="A51" t="s">
+        <v>112</v>
+      </c>
+      <c r="C51" t="s">
+        <v>37</v>
+      </c>
+      <c r="D51" t="s">
+        <v>37</v>
+      </c>
+      <c r="E51" t="s">
+        <v>37</v>
+      </c>
+      <c r="I51" t="s">
+        <v>37</v>
+      </c>
+      <c r="J51" t="s">
+        <v>37</v>
+      </c>
+      <c r="K51" t="s">
+        <v>37</v>
+      </c>
+      <c r="N51" t="s">
+        <v>37</v>
+      </c>
+      <c r="O51" t="s">
+        <v>37</v>
+      </c>
+      <c r="R51" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK51">
+        <v>9</v>
+      </c>
+      <c r="AL51" t="s">
+        <v>44</v>
+      </c>
+      <c r="AM51" s="1">
+        <v>43451</v>
+      </c>
+    </row>
+    <row r="52" spans="1:39">
+      <c r="A52" t="s">
+        <v>113</v>
+      </c>
+      <c r="C52" t="s">
+        <v>37</v>
+      </c>
+      <c r="D52" t="s">
+        <v>37</v>
+      </c>
+      <c r="E52" t="s">
+        <v>37</v>
+      </c>
+      <c r="I52" t="s">
+        <v>37</v>
+      </c>
+      <c r="K52" t="s">
+        <v>37</v>
+      </c>
+      <c r="N52" t="s">
+        <v>37</v>
+      </c>
+      <c r="O52" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q52" t="s">
+        <v>37</v>
+      </c>
+      <c r="S52" t="s">
+        <v>37</v>
+      </c>
+      <c r="T52" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK52">
+        <v>10</v>
+      </c>
+      <c r="AL52" t="s">
+        <v>44</v>
+      </c>
+      <c r="AM52" s="1">
+        <v>43451</v>
+      </c>
+    </row>
+    <row r="53" spans="1:39">
+      <c r="A53" t="s">
+        <v>114</v>
+      </c>
+      <c r="C53" t="s">
+        <v>37</v>
+      </c>
+      <c r="D53" t="s">
+        <v>37</v>
+      </c>
+      <c r="E53" t="s">
+        <v>37</v>
+      </c>
+      <c r="I53" t="s">
+        <v>37</v>
+      </c>
+      <c r="J53" t="s">
+        <v>37</v>
+      </c>
+      <c r="K53" t="s">
+        <v>37</v>
+      </c>
+      <c r="O53" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q53" t="s">
+        <v>37</v>
+      </c>
+      <c r="U53" t="s">
+        <v>37</v>
+      </c>
+      <c r="V53" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK53">
+        <v>10</v>
+      </c>
+      <c r="AL53" t="s">
+        <v>44</v>
+      </c>
+      <c r="AM53" s="1">
+        <v>43451</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add 12/18 and 12/19 ballots
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -9,6 +9,7 @@
   <sheets>
     <sheet name="ballots" sheetId="1" r:id="rId1"/>
     <sheet name="players" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1476" uniqueCount="136">
   <si>
     <t>Roy Halladay</t>
   </si>
@@ -365,6 +366,69 @@
   </si>
   <si>
     <t>Mike Vaccaro</t>
+  </si>
+  <si>
+    <t>Sam Mellinger</t>
+  </si>
+  <si>
+    <t>Jim Reeves</t>
+  </si>
+  <si>
+    <t>Pressbox DFW</t>
+  </si>
+  <si>
+    <t>Ken Rosenthal</t>
+  </si>
+  <si>
+    <t>The Athletic</t>
+  </si>
+  <si>
+    <t>Michael Silverman</t>
+  </si>
+  <si>
+    <t>Boston Herald</t>
+  </si>
+  <si>
+    <t>Clark Spencer</t>
+  </si>
+  <si>
+    <t>Anthony Andro</t>
+  </si>
+  <si>
+    <t>Peter Botte</t>
+  </si>
+  <si>
+    <t>Twiter</t>
+  </si>
+  <si>
+    <t>René Cárdenas (first time public)</t>
+  </si>
+  <si>
+    <t>Kevin Cooney</t>
+  </si>
+  <si>
+    <t>Tony DeMarco</t>
+  </si>
+  <si>
+    <t>Jeffrey Flanagan</t>
+  </si>
+  <si>
+    <t>Jay Greenberg</t>
+  </si>
+  <si>
+    <t>Karen Guregian</t>
+  </si>
+  <si>
+    <t>Bob Klapisch</t>
+  </si>
+  <si>
+    <t>Gil LeBreton (did not vote last yr)</t>
+  </si>
+  <si>
+    <t>Newsday Column</t>
+  </si>
+  <si>
+    <t>Gil LeBreton</t>
   </si>
 </sst>
 </file>
@@ -413,7 +477,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="16">
+  <cellStyleXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -430,12 +494,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="16">
+  <cellStyles count="20">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -444,6 +512,8 @@
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -451,6 +521,8 @@
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="16" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="18" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -780,13 +852,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AM53"/>
+  <dimension ref="A1:AM67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B30" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B40" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A53" sqref="A53"/>
+      <selection pane="bottomRight" activeCell="A68" sqref="A68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2992,6 +3064,565 @@
       </c>
       <c r="AM53" s="1">
         <v>43451</v>
+      </c>
+    </row>
+    <row r="54" spans="1:39">
+      <c r="A54" t="s">
+        <v>115</v>
+      </c>
+      <c r="C54" t="s">
+        <v>37</v>
+      </c>
+      <c r="D54" t="s">
+        <v>37</v>
+      </c>
+      <c r="E54" t="s">
+        <v>37</v>
+      </c>
+      <c r="I54" t="s">
+        <v>37</v>
+      </c>
+      <c r="K54" t="s">
+        <v>37</v>
+      </c>
+      <c r="N54" t="s">
+        <v>37</v>
+      </c>
+      <c r="O54" t="s">
+        <v>37</v>
+      </c>
+      <c r="P54" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q54" t="s">
+        <v>37</v>
+      </c>
+      <c r="V54" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK54">
+        <v>10</v>
+      </c>
+      <c r="AL54" t="s">
+        <v>44</v>
+      </c>
+      <c r="AM54" s="1">
+        <v>43453</v>
+      </c>
+    </row>
+    <row r="55" spans="1:39">
+      <c r="A55" t="s">
+        <v>116</v>
+      </c>
+      <c r="E55" t="s">
+        <v>37</v>
+      </c>
+      <c r="I55" t="s">
+        <v>37</v>
+      </c>
+      <c r="J55" t="s">
+        <v>37</v>
+      </c>
+      <c r="K55" t="s">
+        <v>37</v>
+      </c>
+      <c r="O55" t="s">
+        <v>37</v>
+      </c>
+      <c r="V55" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK55">
+        <v>6</v>
+      </c>
+      <c r="AL55" t="s">
+        <v>117</v>
+      </c>
+      <c r="AM55" s="1">
+        <v>43453</v>
+      </c>
+    </row>
+    <row r="56" spans="1:39">
+      <c r="A56" t="s">
+        <v>118</v>
+      </c>
+      <c r="C56" t="s">
+        <v>37</v>
+      </c>
+      <c r="D56" t="s">
+        <v>37</v>
+      </c>
+      <c r="E56" t="s">
+        <v>37</v>
+      </c>
+      <c r="I56" t="s">
+        <v>37</v>
+      </c>
+      <c r="J56" t="s">
+        <v>37</v>
+      </c>
+      <c r="K56" t="s">
+        <v>37</v>
+      </c>
+      <c r="O56" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q56" t="s">
+        <v>37</v>
+      </c>
+      <c r="U56" t="s">
+        <v>37</v>
+      </c>
+      <c r="V56" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK56">
+        <v>10</v>
+      </c>
+      <c r="AL56" t="s">
+        <v>119</v>
+      </c>
+      <c r="AM56" s="1">
+        <v>43453</v>
+      </c>
+    </row>
+    <row r="57" spans="1:39">
+      <c r="A57" t="s">
+        <v>123</v>
+      </c>
+      <c r="C57" t="s">
+        <v>37</v>
+      </c>
+      <c r="D57" t="s">
+        <v>37</v>
+      </c>
+      <c r="E57" t="s">
+        <v>37</v>
+      </c>
+      <c r="I57" t="s">
+        <v>37</v>
+      </c>
+      <c r="J57" t="s">
+        <v>37</v>
+      </c>
+      <c r="K57" t="s">
+        <v>37</v>
+      </c>
+      <c r="O57" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q57" t="s">
+        <v>37</v>
+      </c>
+      <c r="R57" t="s">
+        <v>37</v>
+      </c>
+      <c r="V57" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK57">
+        <v>10</v>
+      </c>
+      <c r="AL57" t="s">
+        <v>117</v>
+      </c>
+      <c r="AM57" s="1">
+        <v>43453</v>
+      </c>
+    </row>
+    <row r="58" spans="1:39">
+      <c r="A58" t="s">
+        <v>124</v>
+      </c>
+      <c r="C58" t="s">
+        <v>37</v>
+      </c>
+      <c r="D58" t="s">
+        <v>37</v>
+      </c>
+      <c r="E58" t="s">
+        <v>37</v>
+      </c>
+      <c r="H58" t="s">
+        <v>37</v>
+      </c>
+      <c r="I58" t="s">
+        <v>37</v>
+      </c>
+      <c r="J58" t="s">
+        <v>37</v>
+      </c>
+      <c r="O58" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q58" t="s">
+        <v>37</v>
+      </c>
+      <c r="T58" t="s">
+        <v>37</v>
+      </c>
+      <c r="V58" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK58">
+        <v>10</v>
+      </c>
+      <c r="AL58" t="s">
+        <v>125</v>
+      </c>
+      <c r="AM58" s="1">
+        <v>43453</v>
+      </c>
+    </row>
+    <row r="59" spans="1:39">
+      <c r="A59" t="s">
+        <v>128</v>
+      </c>
+      <c r="E59" t="s">
+        <v>37</v>
+      </c>
+      <c r="F59" t="s">
+        <v>37</v>
+      </c>
+      <c r="I59" t="s">
+        <v>37</v>
+      </c>
+      <c r="J59" t="s">
+        <v>37</v>
+      </c>
+      <c r="K59" t="s">
+        <v>37</v>
+      </c>
+      <c r="O59" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q59" t="s">
+        <v>37</v>
+      </c>
+      <c r="T59" t="s">
+        <v>37</v>
+      </c>
+      <c r="V59" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK59">
+        <v>9</v>
+      </c>
+      <c r="AL59" t="s">
+        <v>44</v>
+      </c>
+      <c r="AM59" s="1">
+        <v>43453</v>
+      </c>
+    </row>
+    <row r="60" spans="1:39">
+      <c r="A60" t="s">
+        <v>129</v>
+      </c>
+      <c r="C60" t="s">
+        <v>37</v>
+      </c>
+      <c r="D60" t="s">
+        <v>37</v>
+      </c>
+      <c r="E60" t="s">
+        <v>37</v>
+      </c>
+      <c r="G60" t="s">
+        <v>37</v>
+      </c>
+      <c r="I60" t="s">
+        <v>37</v>
+      </c>
+      <c r="K60" t="s">
+        <v>37</v>
+      </c>
+      <c r="N60" t="s">
+        <v>37</v>
+      </c>
+      <c r="O60" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q60" t="s">
+        <v>37</v>
+      </c>
+      <c r="V60" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK60">
+        <v>10</v>
+      </c>
+      <c r="AL60" t="s">
+        <v>44</v>
+      </c>
+      <c r="AM60" s="1">
+        <v>43453</v>
+      </c>
+    </row>
+    <row r="61" spans="1:39">
+      <c r="A61" t="s">
+        <v>130</v>
+      </c>
+      <c r="E61" t="s">
+        <v>37</v>
+      </c>
+      <c r="I61" t="s">
+        <v>37</v>
+      </c>
+      <c r="K61" t="s">
+        <v>37</v>
+      </c>
+      <c r="O61" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q61" t="s">
+        <v>37</v>
+      </c>
+      <c r="T61" t="s">
+        <v>37</v>
+      </c>
+      <c r="U61" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK61">
+        <v>7</v>
+      </c>
+      <c r="AL61" t="s">
+        <v>44</v>
+      </c>
+      <c r="AM61" s="1">
+        <v>43453</v>
+      </c>
+    </row>
+    <row r="62" spans="1:39">
+      <c r="A62" t="s">
+        <v>135</v>
+      </c>
+      <c r="C62" t="s">
+        <v>37</v>
+      </c>
+      <c r="D62" t="s">
+        <v>37</v>
+      </c>
+      <c r="E62" t="s">
+        <v>37</v>
+      </c>
+      <c r="I62" t="s">
+        <v>37</v>
+      </c>
+      <c r="K62" t="s">
+        <v>37</v>
+      </c>
+      <c r="N62" t="s">
+        <v>37</v>
+      </c>
+      <c r="O62" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q62" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK62">
+        <v>8</v>
+      </c>
+      <c r="AL62" t="s">
+        <v>117</v>
+      </c>
+      <c r="AM62" s="1">
+        <v>43453</v>
+      </c>
+    </row>
+    <row r="63" spans="1:39">
+      <c r="A63" t="s">
+        <v>120</v>
+      </c>
+      <c r="C63" t="s">
+        <v>37</v>
+      </c>
+      <c r="D63" t="s">
+        <v>37</v>
+      </c>
+      <c r="E63" t="s">
+        <v>37</v>
+      </c>
+      <c r="I63" t="s">
+        <v>37</v>
+      </c>
+      <c r="K63" t="s">
+        <v>37</v>
+      </c>
+      <c r="N63" t="s">
+        <v>37</v>
+      </c>
+      <c r="O63" t="s">
+        <v>37</v>
+      </c>
+      <c r="P63" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q63" t="s">
+        <v>37</v>
+      </c>
+      <c r="V63" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK63">
+        <v>10</v>
+      </c>
+      <c r="AL63" t="s">
+        <v>121</v>
+      </c>
+      <c r="AM63" s="1">
+        <v>43452</v>
+      </c>
+    </row>
+    <row r="64" spans="1:39">
+      <c r="A64" t="s">
+        <v>122</v>
+      </c>
+      <c r="E64" t="s">
+        <v>37</v>
+      </c>
+      <c r="I64" t="s">
+        <v>37</v>
+      </c>
+      <c r="K64" t="s">
+        <v>37</v>
+      </c>
+      <c r="O64" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q64" t="s">
+        <v>37</v>
+      </c>
+      <c r="V64" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK64">
+        <v>6</v>
+      </c>
+      <c r="AL64" t="s">
+        <v>44</v>
+      </c>
+      <c r="AM64" s="1">
+        <v>43452</v>
+      </c>
+    </row>
+    <row r="65" spans="1:39">
+      <c r="A65" t="s">
+        <v>127</v>
+      </c>
+      <c r="C65" t="s">
+        <v>37</v>
+      </c>
+      <c r="D65" t="s">
+        <v>37</v>
+      </c>
+      <c r="E65" t="s">
+        <v>37</v>
+      </c>
+      <c r="I65" t="s">
+        <v>37</v>
+      </c>
+      <c r="J65" t="s">
+        <v>37</v>
+      </c>
+      <c r="K65" t="s">
+        <v>37</v>
+      </c>
+      <c r="O65" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q65" t="s">
+        <v>37</v>
+      </c>
+      <c r="T65" t="s">
+        <v>37</v>
+      </c>
+      <c r="U65" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK65">
+        <v>10</v>
+      </c>
+      <c r="AL65" t="s">
+        <v>44</v>
+      </c>
+      <c r="AM65" s="1">
+        <v>43452</v>
+      </c>
+    </row>
+    <row r="66" spans="1:39">
+      <c r="A66" t="s">
+        <v>131</v>
+      </c>
+      <c r="I66" t="s">
+        <v>37</v>
+      </c>
+      <c r="K66" t="s">
+        <v>37</v>
+      </c>
+      <c r="O66" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q66" t="s">
+        <v>37</v>
+      </c>
+      <c r="T66" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK66">
+        <v>5</v>
+      </c>
+      <c r="AL66" t="s">
+        <v>38</v>
+      </c>
+      <c r="AM66" s="1">
+        <v>43452</v>
+      </c>
+    </row>
+    <row r="67" spans="1:39">
+      <c r="A67" t="s">
+        <v>132</v>
+      </c>
+      <c r="C67" t="s">
+        <v>37</v>
+      </c>
+      <c r="D67" t="s">
+        <v>37</v>
+      </c>
+      <c r="E67" t="s">
+        <v>37</v>
+      </c>
+      <c r="I67" t="s">
+        <v>37</v>
+      </c>
+      <c r="J67" t="s">
+        <v>37</v>
+      </c>
+      <c r="K67" t="s">
+        <v>37</v>
+      </c>
+      <c r="O67" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q67" t="s">
+        <v>37</v>
+      </c>
+      <c r="T67" t="s">
+        <v>37</v>
+      </c>
+      <c r="V67" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK67">
+        <v>10</v>
+      </c>
+      <c r="AL67" t="s">
+        <v>44</v>
+      </c>
+      <c r="AM67" s="1">
+        <v>43452</v>
       </c>
     </row>
   </sheetData>
@@ -3315,4 +3946,2633 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AM65"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A1:XFD14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:39">
+      <c r="A1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K1" t="s">
+        <v>37</v>
+      </c>
+      <c r="N1" t="s">
+        <v>37</v>
+      </c>
+      <c r="O1" t="s">
+        <v>37</v>
+      </c>
+      <c r="P1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK1">
+        <v>10</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AM1" s="1">
+        <v>43453</v>
+      </c>
+    </row>
+    <row r="2" spans="1:39">
+      <c r="A2" t="s">
+        <v>116</v>
+      </c>
+      <c r="E2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J2" t="s">
+        <v>37</v>
+      </c>
+      <c r="K2" t="s">
+        <v>37</v>
+      </c>
+      <c r="O2" t="s">
+        <v>37</v>
+      </c>
+      <c r="V2" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK2">
+        <v>6</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>117</v>
+      </c>
+      <c r="AM2" s="1">
+        <v>43453</v>
+      </c>
+    </row>
+    <row r="3" spans="1:39">
+      <c r="A3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I3" t="s">
+        <v>37</v>
+      </c>
+      <c r="J3" t="s">
+        <v>37</v>
+      </c>
+      <c r="K3" t="s">
+        <v>37</v>
+      </c>
+      <c r="O3" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>37</v>
+      </c>
+      <c r="U3" t="s">
+        <v>37</v>
+      </c>
+      <c r="V3" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK3">
+        <v>10</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>119</v>
+      </c>
+      <c r="AM3" s="1">
+        <v>43453</v>
+      </c>
+    </row>
+    <row r="4" spans="1:39">
+      <c r="A4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" t="s">
+        <v>37</v>
+      </c>
+      <c r="I4" t="s">
+        <v>37</v>
+      </c>
+      <c r="J4" t="s">
+        <v>37</v>
+      </c>
+      <c r="K4" t="s">
+        <v>37</v>
+      </c>
+      <c r="O4" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>37</v>
+      </c>
+      <c r="R4" t="s">
+        <v>37</v>
+      </c>
+      <c r="V4" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK4">
+        <v>10</v>
+      </c>
+      <c r="AL4" t="s">
+        <v>117</v>
+      </c>
+      <c r="AM4" s="1">
+        <v>43453</v>
+      </c>
+    </row>
+    <row r="5" spans="1:39">
+      <c r="A5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5" t="s">
+        <v>37</v>
+      </c>
+      <c r="I5" t="s">
+        <v>37</v>
+      </c>
+      <c r="J5" t="s">
+        <v>37</v>
+      </c>
+      <c r="O5" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>37</v>
+      </c>
+      <c r="T5" t="s">
+        <v>37</v>
+      </c>
+      <c r="V5" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK5">
+        <v>10</v>
+      </c>
+      <c r="AL5" t="s">
+        <v>125</v>
+      </c>
+      <c r="AM5" s="1">
+        <v>43453</v>
+      </c>
+    </row>
+    <row r="6" spans="1:39">
+      <c r="A6" t="s">
+        <v>128</v>
+      </c>
+      <c r="E6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" t="s">
+        <v>37</v>
+      </c>
+      <c r="I6" t="s">
+        <v>37</v>
+      </c>
+      <c r="J6" t="s">
+        <v>37</v>
+      </c>
+      <c r="K6" t="s">
+        <v>37</v>
+      </c>
+      <c r="O6" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>37</v>
+      </c>
+      <c r="T6" t="s">
+        <v>37</v>
+      </c>
+      <c r="V6" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK6">
+        <v>9</v>
+      </c>
+      <c r="AL6" t="s">
+        <v>44</v>
+      </c>
+      <c r="AM6" s="1">
+        <v>43453</v>
+      </c>
+    </row>
+    <row r="7" spans="1:39">
+      <c r="A7" t="s">
+        <v>129</v>
+      </c>
+      <c r="C7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G7" t="s">
+        <v>37</v>
+      </c>
+      <c r="I7" t="s">
+        <v>37</v>
+      </c>
+      <c r="K7" t="s">
+        <v>37</v>
+      </c>
+      <c r="N7" t="s">
+        <v>37</v>
+      </c>
+      <c r="O7" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>37</v>
+      </c>
+      <c r="V7" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK7">
+        <v>10</v>
+      </c>
+      <c r="AL7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AM7" s="1">
+        <v>43453</v>
+      </c>
+    </row>
+    <row r="8" spans="1:39">
+      <c r="A8" t="s">
+        <v>130</v>
+      </c>
+      <c r="E8" t="s">
+        <v>37</v>
+      </c>
+      <c r="I8" t="s">
+        <v>37</v>
+      </c>
+      <c r="K8" t="s">
+        <v>37</v>
+      </c>
+      <c r="O8" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>37</v>
+      </c>
+      <c r="T8" t="s">
+        <v>37</v>
+      </c>
+      <c r="U8" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK8">
+        <v>7</v>
+      </c>
+      <c r="AL8" t="s">
+        <v>44</v>
+      </c>
+      <c r="AM8" s="1">
+        <v>43453</v>
+      </c>
+    </row>
+    <row r="9" spans="1:39">
+      <c r="A9" t="s">
+        <v>133</v>
+      </c>
+      <c r="C9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" t="s">
+        <v>37</v>
+      </c>
+      <c r="I9" t="s">
+        <v>37</v>
+      </c>
+      <c r="K9" t="s">
+        <v>37</v>
+      </c>
+      <c r="N9" t="s">
+        <v>37</v>
+      </c>
+      <c r="O9" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK9">
+        <v>8</v>
+      </c>
+      <c r="AL9" t="s">
+        <v>117</v>
+      </c>
+      <c r="AM9" s="1">
+        <v>43453</v>
+      </c>
+    </row>
+    <row r="10" spans="1:39">
+      <c r="A10" t="s">
+        <v>120</v>
+      </c>
+      <c r="C10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" t="s">
+        <v>37</v>
+      </c>
+      <c r="I10" t="s">
+        <v>37</v>
+      </c>
+      <c r="K10" t="s">
+        <v>37</v>
+      </c>
+      <c r="N10" t="s">
+        <v>37</v>
+      </c>
+      <c r="O10" t="s">
+        <v>37</v>
+      </c>
+      <c r="P10" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>37</v>
+      </c>
+      <c r="V10" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK10">
+        <v>10</v>
+      </c>
+      <c r="AL10" t="s">
+        <v>121</v>
+      </c>
+      <c r="AM10" s="1">
+        <v>43452</v>
+      </c>
+    </row>
+    <row r="11" spans="1:39">
+      <c r="A11" t="s">
+        <v>122</v>
+      </c>
+      <c r="E11" t="s">
+        <v>37</v>
+      </c>
+      <c r="I11" t="s">
+        <v>37</v>
+      </c>
+      <c r="K11" t="s">
+        <v>37</v>
+      </c>
+      <c r="O11" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>37</v>
+      </c>
+      <c r="V11" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK11">
+        <v>6</v>
+      </c>
+      <c r="AL11" t="s">
+        <v>44</v>
+      </c>
+      <c r="AM11" s="1">
+        <v>43452</v>
+      </c>
+    </row>
+    <row r="12" spans="1:39">
+      <c r="A12" t="s">
+        <v>127</v>
+      </c>
+      <c r="C12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" t="s">
+        <v>37</v>
+      </c>
+      <c r="I12" t="s">
+        <v>37</v>
+      </c>
+      <c r="J12" t="s">
+        <v>37</v>
+      </c>
+      <c r="K12" t="s">
+        <v>37</v>
+      </c>
+      <c r="O12" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>37</v>
+      </c>
+      <c r="T12" t="s">
+        <v>37</v>
+      </c>
+      <c r="U12" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK12">
+        <v>10</v>
+      </c>
+      <c r="AL12" t="s">
+        <v>44</v>
+      </c>
+      <c r="AM12" s="1">
+        <v>43452</v>
+      </c>
+    </row>
+    <row r="13" spans="1:39">
+      <c r="A13" t="s">
+        <v>131</v>
+      </c>
+      <c r="I13" t="s">
+        <v>37</v>
+      </c>
+      <c r="K13" t="s">
+        <v>37</v>
+      </c>
+      <c r="O13" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>37</v>
+      </c>
+      <c r="T13" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK13">
+        <v>5</v>
+      </c>
+      <c r="AL13" t="s">
+        <v>38</v>
+      </c>
+      <c r="AM13" s="1">
+        <v>43452</v>
+      </c>
+    </row>
+    <row r="14" spans="1:39">
+      <c r="A14" t="s">
+        <v>132</v>
+      </c>
+      <c r="C14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" t="s">
+        <v>37</v>
+      </c>
+      <c r="I14" t="s">
+        <v>37</v>
+      </c>
+      <c r="J14" t="s">
+        <v>37</v>
+      </c>
+      <c r="K14" t="s">
+        <v>37</v>
+      </c>
+      <c r="O14" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>37</v>
+      </c>
+      <c r="T14" t="s">
+        <v>37</v>
+      </c>
+      <c r="V14" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK14">
+        <v>10</v>
+      </c>
+      <c r="AL14" t="s">
+        <v>44</v>
+      </c>
+      <c r="AM14" s="1">
+        <v>43452</v>
+      </c>
+    </row>
+    <row r="15" spans="1:39">
+      <c r="A15" t="s">
+        <v>114</v>
+      </c>
+      <c r="C15" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" t="s">
+        <v>37</v>
+      </c>
+      <c r="E15" t="s">
+        <v>37</v>
+      </c>
+      <c r="I15" t="s">
+        <v>37</v>
+      </c>
+      <c r="J15" t="s">
+        <v>37</v>
+      </c>
+      <c r="K15" t="s">
+        <v>37</v>
+      </c>
+      <c r="O15" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>37</v>
+      </c>
+      <c r="U15" t="s">
+        <v>37</v>
+      </c>
+      <c r="V15" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK15">
+        <v>10</v>
+      </c>
+      <c r="AL15" t="s">
+        <v>44</v>
+      </c>
+      <c r="AM15" s="1">
+        <v>43451</v>
+      </c>
+    </row>
+    <row r="16" spans="1:39">
+      <c r="A16" t="s">
+        <v>110</v>
+      </c>
+      <c r="C16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" t="s">
+        <v>37</v>
+      </c>
+      <c r="I16" t="s">
+        <v>37</v>
+      </c>
+      <c r="J16" t="s">
+        <v>37</v>
+      </c>
+      <c r="K16" t="s">
+        <v>37</v>
+      </c>
+      <c r="O16" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>37</v>
+      </c>
+      <c r="S16" t="s">
+        <v>37</v>
+      </c>
+      <c r="T16" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK16">
+        <v>10</v>
+      </c>
+      <c r="AL16" t="s">
+        <v>111</v>
+      </c>
+      <c r="AM16" s="1">
+        <v>43451</v>
+      </c>
+    </row>
+    <row r="17" spans="1:39">
+      <c r="A17" t="s">
+        <v>112</v>
+      </c>
+      <c r="C17" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17" t="s">
+        <v>37</v>
+      </c>
+      <c r="I17" t="s">
+        <v>37</v>
+      </c>
+      <c r="J17" t="s">
+        <v>37</v>
+      </c>
+      <c r="K17" t="s">
+        <v>37</v>
+      </c>
+      <c r="N17" t="s">
+        <v>37</v>
+      </c>
+      <c r="O17" t="s">
+        <v>37</v>
+      </c>
+      <c r="R17" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK17">
+        <v>9</v>
+      </c>
+      <c r="AL17" t="s">
+        <v>44</v>
+      </c>
+      <c r="AM17" s="1">
+        <v>43451</v>
+      </c>
+    </row>
+    <row r="18" spans="1:39">
+      <c r="A18" t="s">
+        <v>113</v>
+      </c>
+      <c r="C18" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" t="s">
+        <v>37</v>
+      </c>
+      <c r="E18" t="s">
+        <v>37</v>
+      </c>
+      <c r="I18" t="s">
+        <v>37</v>
+      </c>
+      <c r="K18" t="s">
+        <v>37</v>
+      </c>
+      <c r="N18" t="s">
+        <v>37</v>
+      </c>
+      <c r="O18" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>37</v>
+      </c>
+      <c r="S18" t="s">
+        <v>37</v>
+      </c>
+      <c r="T18" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK18">
+        <v>10</v>
+      </c>
+      <c r="AL18" t="s">
+        <v>44</v>
+      </c>
+      <c r="AM18" s="1">
+        <v>43451</v>
+      </c>
+    </row>
+    <row r="19" spans="1:39">
+      <c r="A19" t="s">
+        <v>106</v>
+      </c>
+      <c r="C19" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" t="s">
+        <v>37</v>
+      </c>
+      <c r="E19" t="s">
+        <v>37</v>
+      </c>
+      <c r="I19" t="s">
+        <v>37</v>
+      </c>
+      <c r="K19" t="s">
+        <v>37</v>
+      </c>
+      <c r="M19" t="s">
+        <v>37</v>
+      </c>
+      <c r="O19" t="s">
+        <v>37</v>
+      </c>
+      <c r="P19" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>37</v>
+      </c>
+      <c r="V19" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK19">
+        <v>10</v>
+      </c>
+      <c r="AL19" t="s">
+        <v>44</v>
+      </c>
+      <c r="AM19" s="1">
+        <v>43450</v>
+      </c>
+    </row>
+    <row r="20" spans="1:39">
+      <c r="A20" t="s">
+        <v>109</v>
+      </c>
+      <c r="C20" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" t="s">
+        <v>37</v>
+      </c>
+      <c r="E20" t="s">
+        <v>37</v>
+      </c>
+      <c r="O20" t="s">
+        <v>37</v>
+      </c>
+      <c r="V20" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK20">
+        <v>5</v>
+      </c>
+      <c r="AL20" t="s">
+        <v>44</v>
+      </c>
+      <c r="AM20" s="1">
+        <v>43449</v>
+      </c>
+    </row>
+    <row r="21" spans="1:39">
+      <c r="A21" t="s">
+        <v>108</v>
+      </c>
+      <c r="C21" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21" t="s">
+        <v>37</v>
+      </c>
+      <c r="E21" t="s">
+        <v>37</v>
+      </c>
+      <c r="I21" t="s">
+        <v>37</v>
+      </c>
+      <c r="K21" t="s">
+        <v>37</v>
+      </c>
+      <c r="N21" t="s">
+        <v>37</v>
+      </c>
+      <c r="O21" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>37</v>
+      </c>
+      <c r="V21" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK21">
+        <v>9</v>
+      </c>
+      <c r="AL21" t="s">
+        <v>44</v>
+      </c>
+      <c r="AM21" s="1">
+        <v>43449</v>
+      </c>
+    </row>
+    <row r="22" spans="1:39">
+      <c r="A22" t="s">
+        <v>107</v>
+      </c>
+      <c r="C22" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" t="s">
+        <v>37</v>
+      </c>
+      <c r="E22" t="s">
+        <v>37</v>
+      </c>
+      <c r="I22" t="s">
+        <v>37</v>
+      </c>
+      <c r="K22" t="s">
+        <v>37</v>
+      </c>
+      <c r="O22" t="s">
+        <v>37</v>
+      </c>
+      <c r="P22" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>37</v>
+      </c>
+      <c r="U22" t="s">
+        <v>37</v>
+      </c>
+      <c r="V22" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK22">
+        <v>10</v>
+      </c>
+      <c r="AL22" t="s">
+        <v>38</v>
+      </c>
+      <c r="AM22" s="1">
+        <v>43449</v>
+      </c>
+    </row>
+    <row r="23" spans="1:39">
+      <c r="A23" t="s">
+        <v>103</v>
+      </c>
+      <c r="C23" t="s">
+        <v>37</v>
+      </c>
+      <c r="D23" t="s">
+        <v>37</v>
+      </c>
+      <c r="E23" t="s">
+        <v>37</v>
+      </c>
+      <c r="I23" t="s">
+        <v>37</v>
+      </c>
+      <c r="O23" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK23">
+        <v>6</v>
+      </c>
+      <c r="AL23" t="s">
+        <v>104</v>
+      </c>
+      <c r="AM23" s="1">
+        <v>43448</v>
+      </c>
+    </row>
+    <row r="24" spans="1:39">
+      <c r="A24" t="s">
+        <v>105</v>
+      </c>
+      <c r="C24" t="s">
+        <v>37</v>
+      </c>
+      <c r="D24" t="s">
+        <v>37</v>
+      </c>
+      <c r="E24" t="s">
+        <v>37</v>
+      </c>
+      <c r="H24" t="s">
+        <v>37</v>
+      </c>
+      <c r="I24" t="s">
+        <v>37</v>
+      </c>
+      <c r="K24" t="s">
+        <v>37</v>
+      </c>
+      <c r="O24" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>37</v>
+      </c>
+      <c r="T24" t="s">
+        <v>37</v>
+      </c>
+      <c r="V24" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK24">
+        <v>10</v>
+      </c>
+      <c r="AL24" t="s">
+        <v>44</v>
+      </c>
+      <c r="AM24" s="1">
+        <v>43448</v>
+      </c>
+    </row>
+    <row r="25" spans="1:39">
+      <c r="A25" t="s">
+        <v>101</v>
+      </c>
+      <c r="C25" t="s">
+        <v>37</v>
+      </c>
+      <c r="D25" t="s">
+        <v>37</v>
+      </c>
+      <c r="E25" t="s">
+        <v>37</v>
+      </c>
+      <c r="I25" t="s">
+        <v>37</v>
+      </c>
+      <c r="K25" t="s">
+        <v>37</v>
+      </c>
+      <c r="N25" t="s">
+        <v>37</v>
+      </c>
+      <c r="O25" t="s">
+        <v>37</v>
+      </c>
+      <c r="P25" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>37</v>
+      </c>
+      <c r="V25" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK25">
+        <v>10</v>
+      </c>
+      <c r="AL25" t="s">
+        <v>102</v>
+      </c>
+      <c r="AM25" s="1">
+        <v>43448</v>
+      </c>
+    </row>
+    <row r="26" spans="1:39">
+      <c r="A26" t="s">
+        <v>100</v>
+      </c>
+      <c r="C26" t="s">
+        <v>37</v>
+      </c>
+      <c r="D26" t="s">
+        <v>37</v>
+      </c>
+      <c r="O26" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK26">
+        <v>3</v>
+      </c>
+      <c r="AL26" t="s">
+        <v>134</v>
+      </c>
+      <c r="AM26" s="1">
+        <v>43448</v>
+      </c>
+    </row>
+    <row r="27" spans="1:39">
+      <c r="A27" t="s">
+        <v>91</v>
+      </c>
+      <c r="F27" t="s">
+        <v>37</v>
+      </c>
+      <c r="J27" t="s">
+        <v>37</v>
+      </c>
+      <c r="K27" t="s">
+        <v>37</v>
+      </c>
+      <c r="M27" t="s">
+        <v>37</v>
+      </c>
+      <c r="O27" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK27">
+        <v>5</v>
+      </c>
+      <c r="AL27" t="s">
+        <v>92</v>
+      </c>
+      <c r="AM27" s="1">
+        <v>43447</v>
+      </c>
+    </row>
+    <row r="28" spans="1:39">
+      <c r="A28" t="s">
+        <v>93</v>
+      </c>
+      <c r="E28" t="s">
+        <v>37</v>
+      </c>
+      <c r="K28" t="s">
+        <v>37</v>
+      </c>
+      <c r="O28" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>37</v>
+      </c>
+      <c r="V28" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK28">
+        <v>5</v>
+      </c>
+      <c r="AL28" t="s">
+        <v>44</v>
+      </c>
+      <c r="AM28" s="1">
+        <v>43447</v>
+      </c>
+    </row>
+    <row r="29" spans="1:39">
+      <c r="A29" t="s">
+        <v>95</v>
+      </c>
+      <c r="E29" t="s">
+        <v>37</v>
+      </c>
+      <c r="F29" t="s">
+        <v>37</v>
+      </c>
+      <c r="I29" t="s">
+        <v>37</v>
+      </c>
+      <c r="J29" t="s">
+        <v>37</v>
+      </c>
+      <c r="K29" t="s">
+        <v>37</v>
+      </c>
+      <c r="O29" t="s">
+        <v>37</v>
+      </c>
+      <c r="P29" t="s">
+        <v>37</v>
+      </c>
+      <c r="V29" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK29">
+        <v>8</v>
+      </c>
+      <c r="AL29" t="s">
+        <v>70</v>
+      </c>
+      <c r="AM29" s="1">
+        <v>43447</v>
+      </c>
+    </row>
+    <row r="30" spans="1:39">
+      <c r="A30" t="s">
+        <v>96</v>
+      </c>
+      <c r="C30" t="s">
+        <v>37</v>
+      </c>
+      <c r="D30" t="s">
+        <v>37</v>
+      </c>
+      <c r="E30" t="s">
+        <v>37</v>
+      </c>
+      <c r="I30" t="s">
+        <v>37</v>
+      </c>
+      <c r="K30" t="s">
+        <v>37</v>
+      </c>
+      <c r="O30" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>37</v>
+      </c>
+      <c r="V30" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK30">
+        <v>8</v>
+      </c>
+      <c r="AL30" t="s">
+        <v>98</v>
+      </c>
+      <c r="AM30" s="1">
+        <v>43447</v>
+      </c>
+    </row>
+    <row r="31" spans="1:39">
+      <c r="A31" t="s">
+        <v>89</v>
+      </c>
+      <c r="C31" t="s">
+        <v>37</v>
+      </c>
+      <c r="D31" t="s">
+        <v>37</v>
+      </c>
+      <c r="E31" t="s">
+        <v>37</v>
+      </c>
+      <c r="F31" t="s">
+        <v>37</v>
+      </c>
+      <c r="I31" t="s">
+        <v>37</v>
+      </c>
+      <c r="K31" t="s">
+        <v>37</v>
+      </c>
+      <c r="O31" t="s">
+        <v>37</v>
+      </c>
+      <c r="P31" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>37</v>
+      </c>
+      <c r="V31" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK31">
+        <v>10</v>
+      </c>
+      <c r="AL31" t="s">
+        <v>44</v>
+      </c>
+      <c r="AM31" s="1">
+        <v>43446</v>
+      </c>
+    </row>
+    <row r="32" spans="1:39">
+      <c r="A32" t="s">
+        <v>90</v>
+      </c>
+      <c r="C32" t="s">
+        <v>37</v>
+      </c>
+      <c r="D32" t="s">
+        <v>37</v>
+      </c>
+      <c r="E32" t="s">
+        <v>37</v>
+      </c>
+      <c r="G32" t="s">
+        <v>37</v>
+      </c>
+      <c r="I32" t="s">
+        <v>37</v>
+      </c>
+      <c r="J32" t="s">
+        <v>37</v>
+      </c>
+      <c r="O32" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>37</v>
+      </c>
+      <c r="T32" t="s">
+        <v>37</v>
+      </c>
+      <c r="V32" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK32">
+        <v>10</v>
+      </c>
+      <c r="AL32" t="s">
+        <v>44</v>
+      </c>
+      <c r="AM32" s="1">
+        <v>43446</v>
+      </c>
+    </row>
+    <row r="33" spans="1:39">
+      <c r="A33" t="s">
+        <v>88</v>
+      </c>
+      <c r="C33" t="s">
+        <v>37</v>
+      </c>
+      <c r="D33" t="s">
+        <v>37</v>
+      </c>
+      <c r="E33" t="s">
+        <v>37</v>
+      </c>
+      <c r="K33" t="s">
+        <v>37</v>
+      </c>
+      <c r="N33" t="s">
+        <v>37</v>
+      </c>
+      <c r="O33" t="s">
+        <v>37</v>
+      </c>
+      <c r="R33" t="s">
+        <v>37</v>
+      </c>
+      <c r="S33" t="s">
+        <v>37</v>
+      </c>
+      <c r="W33" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK33">
+        <v>9</v>
+      </c>
+      <c r="AL33" t="s">
+        <v>38</v>
+      </c>
+      <c r="AM33" s="1">
+        <v>43445</v>
+      </c>
+    </row>
+    <row r="34" spans="1:39">
+      <c r="A34" t="s">
+        <v>84</v>
+      </c>
+      <c r="C34" t="s">
+        <v>37</v>
+      </c>
+      <c r="D34" t="s">
+        <v>37</v>
+      </c>
+      <c r="E34" t="s">
+        <v>37</v>
+      </c>
+      <c r="F34" t="s">
+        <v>37</v>
+      </c>
+      <c r="I34" t="s">
+        <v>37</v>
+      </c>
+      <c r="J34" t="s">
+        <v>37</v>
+      </c>
+      <c r="K34" t="s">
+        <v>37</v>
+      </c>
+      <c r="O34" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>37</v>
+      </c>
+      <c r="V34" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK34">
+        <v>10</v>
+      </c>
+      <c r="AL34" t="s">
+        <v>44</v>
+      </c>
+      <c r="AM34" s="1">
+        <v>43444</v>
+      </c>
+    </row>
+    <row r="35" spans="1:39">
+      <c r="A35" t="s">
+        <v>85</v>
+      </c>
+      <c r="E35" t="s">
+        <v>37</v>
+      </c>
+      <c r="F35" t="s">
+        <v>37</v>
+      </c>
+      <c r="I35" t="s">
+        <v>37</v>
+      </c>
+      <c r="K35" t="s">
+        <v>37</v>
+      </c>
+      <c r="O35" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>37</v>
+      </c>
+      <c r="R35" t="s">
+        <v>37</v>
+      </c>
+      <c r="U35" t="s">
+        <v>37</v>
+      </c>
+      <c r="V35" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK35">
+        <v>9</v>
+      </c>
+      <c r="AL35" t="s">
+        <v>38</v>
+      </c>
+      <c r="AM35" s="1">
+        <v>43444</v>
+      </c>
+    </row>
+    <row r="36" spans="1:39">
+      <c r="A36" t="s">
+        <v>86</v>
+      </c>
+      <c r="C36" t="s">
+        <v>37</v>
+      </c>
+      <c r="D36" t="s">
+        <v>37</v>
+      </c>
+      <c r="E36" t="s">
+        <v>37</v>
+      </c>
+      <c r="I36" t="s">
+        <v>37</v>
+      </c>
+      <c r="J36" t="s">
+        <v>37</v>
+      </c>
+      <c r="K36" t="s">
+        <v>37</v>
+      </c>
+      <c r="O36" t="s">
+        <v>37</v>
+      </c>
+      <c r="P36" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>37</v>
+      </c>
+      <c r="V36" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK36">
+        <v>10</v>
+      </c>
+      <c r="AL36" t="s">
+        <v>44</v>
+      </c>
+      <c r="AM36" s="1">
+        <v>43444</v>
+      </c>
+    </row>
+    <row r="37" spans="1:39">
+      <c r="A37" t="s">
+        <v>82</v>
+      </c>
+      <c r="C37" t="s">
+        <v>37</v>
+      </c>
+      <c r="D37" t="s">
+        <v>37</v>
+      </c>
+      <c r="E37" t="s">
+        <v>37</v>
+      </c>
+      <c r="I37" t="s">
+        <v>37</v>
+      </c>
+      <c r="K37" t="s">
+        <v>37</v>
+      </c>
+      <c r="N37" t="s">
+        <v>37</v>
+      </c>
+      <c r="O37" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>37</v>
+      </c>
+      <c r="R37" t="s">
+        <v>37</v>
+      </c>
+      <c r="S37" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK37">
+        <v>10</v>
+      </c>
+      <c r="AL37" t="s">
+        <v>44</v>
+      </c>
+      <c r="AM37" s="1">
+        <v>43443</v>
+      </c>
+    </row>
+    <row r="38" spans="1:39">
+      <c r="A38" t="s">
+        <v>83</v>
+      </c>
+      <c r="E38" t="s">
+        <v>37</v>
+      </c>
+      <c r="F38" t="s">
+        <v>37</v>
+      </c>
+      <c r="I38" t="s">
+        <v>37</v>
+      </c>
+      <c r="J38" t="s">
+        <v>37</v>
+      </c>
+      <c r="K38" t="s">
+        <v>37</v>
+      </c>
+      <c r="O38" t="s">
+        <v>37</v>
+      </c>
+      <c r="T38" t="s">
+        <v>37</v>
+      </c>
+      <c r="V38" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK38">
+        <v>8</v>
+      </c>
+      <c r="AL38" t="s">
+        <v>70</v>
+      </c>
+      <c r="AM38" s="1">
+        <v>43443</v>
+      </c>
+    </row>
+    <row r="39" spans="1:39">
+      <c r="A39" t="s">
+        <v>81</v>
+      </c>
+      <c r="E39" t="s">
+        <v>37</v>
+      </c>
+      <c r="H39" t="s">
+        <v>37</v>
+      </c>
+      <c r="I39" t="s">
+        <v>37</v>
+      </c>
+      <c r="J39" t="s">
+        <v>37</v>
+      </c>
+      <c r="K39" t="s">
+        <v>37</v>
+      </c>
+      <c r="O39" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>37</v>
+      </c>
+      <c r="T39" t="s">
+        <v>37</v>
+      </c>
+      <c r="V39" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK39">
+        <v>9</v>
+      </c>
+      <c r="AL39" t="s">
+        <v>44</v>
+      </c>
+      <c r="AM39" s="1">
+        <v>43442</v>
+      </c>
+    </row>
+    <row r="40" spans="1:39">
+      <c r="A40" t="s">
+        <v>78</v>
+      </c>
+      <c r="E40" t="s">
+        <v>37</v>
+      </c>
+      <c r="I40" t="s">
+        <v>37</v>
+      </c>
+      <c r="J40" t="s">
+        <v>37</v>
+      </c>
+      <c r="K40" t="s">
+        <v>37</v>
+      </c>
+      <c r="O40" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>37</v>
+      </c>
+      <c r="T40" t="s">
+        <v>37</v>
+      </c>
+      <c r="V40" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK40">
+        <v>8</v>
+      </c>
+      <c r="AL40" t="s">
+        <v>79</v>
+      </c>
+      <c r="AM40" s="1">
+        <v>43442</v>
+      </c>
+    </row>
+    <row r="41" spans="1:39">
+      <c r="A41" t="s">
+        <v>80</v>
+      </c>
+      <c r="C41" t="s">
+        <v>37</v>
+      </c>
+      <c r="D41" t="s">
+        <v>37</v>
+      </c>
+      <c r="E41" t="s">
+        <v>37</v>
+      </c>
+      <c r="H41" t="s">
+        <v>37</v>
+      </c>
+      <c r="I41" t="s">
+        <v>37</v>
+      </c>
+      <c r="K41" t="s">
+        <v>37</v>
+      </c>
+      <c r="O41" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>37</v>
+      </c>
+      <c r="T41" t="s">
+        <v>37</v>
+      </c>
+      <c r="V41" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK41">
+        <v>10</v>
+      </c>
+      <c r="AL41" t="s">
+        <v>44</v>
+      </c>
+      <c r="AM41" s="1">
+        <v>43442</v>
+      </c>
+    </row>
+    <row r="42" spans="1:39">
+      <c r="A42" t="s">
+        <v>74</v>
+      </c>
+      <c r="E42" t="s">
+        <v>37</v>
+      </c>
+      <c r="F42" t="s">
+        <v>37</v>
+      </c>
+      <c r="I42" t="s">
+        <v>37</v>
+      </c>
+      <c r="O42" t="s">
+        <v>37</v>
+      </c>
+      <c r="R42" t="s">
+        <v>37</v>
+      </c>
+      <c r="V42" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK42">
+        <v>6</v>
+      </c>
+      <c r="AL42" t="s">
+        <v>38</v>
+      </c>
+      <c r="AM42" s="1">
+        <v>43441</v>
+      </c>
+    </row>
+    <row r="43" spans="1:39">
+      <c r="A43" t="s">
+        <v>77</v>
+      </c>
+      <c r="C43" t="s">
+        <v>37</v>
+      </c>
+      <c r="D43" t="s">
+        <v>37</v>
+      </c>
+      <c r="E43" t="s">
+        <v>37</v>
+      </c>
+      <c r="F43" t="s">
+        <v>37</v>
+      </c>
+      <c r="I43" t="s">
+        <v>37</v>
+      </c>
+      <c r="K43" t="s">
+        <v>37</v>
+      </c>
+      <c r="O43" t="s">
+        <v>37</v>
+      </c>
+      <c r="P43" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q43" t="s">
+        <v>37</v>
+      </c>
+      <c r="V43" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK43">
+        <v>10</v>
+      </c>
+      <c r="AL43" t="s">
+        <v>44</v>
+      </c>
+      <c r="AM43" s="1">
+        <v>43441</v>
+      </c>
+    </row>
+    <row r="44" spans="1:39">
+      <c r="A44" t="s">
+        <v>126</v>
+      </c>
+      <c r="B44" t="s">
+        <v>37</v>
+      </c>
+      <c r="D44" t="s">
+        <v>37</v>
+      </c>
+      <c r="H44" t="s">
+        <v>37</v>
+      </c>
+      <c r="I44" t="s">
+        <v>37</v>
+      </c>
+      <c r="L44" t="s">
+        <v>37</v>
+      </c>
+      <c r="O44" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q44" t="s">
+        <v>37</v>
+      </c>
+      <c r="T44" t="s">
+        <v>37</v>
+      </c>
+      <c r="U44" t="s">
+        <v>37</v>
+      </c>
+      <c r="V44" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK44">
+        <v>10</v>
+      </c>
+      <c r="AL44" t="s">
+        <v>44</v>
+      </c>
+      <c r="AM44" s="1">
+        <v>43441</v>
+      </c>
+    </row>
+    <row r="45" spans="1:39">
+      <c r="A45" t="s">
+        <v>73</v>
+      </c>
+      <c r="C45" t="s">
+        <v>37</v>
+      </c>
+      <c r="D45" t="s">
+        <v>37</v>
+      </c>
+      <c r="E45" t="s">
+        <v>37</v>
+      </c>
+      <c r="I45" t="s">
+        <v>37</v>
+      </c>
+      <c r="K45" t="s">
+        <v>37</v>
+      </c>
+      <c r="N45" t="s">
+        <v>37</v>
+      </c>
+      <c r="O45" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q45" t="s">
+        <v>37</v>
+      </c>
+      <c r="T45" t="s">
+        <v>37</v>
+      </c>
+      <c r="V45" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK45">
+        <v>10</v>
+      </c>
+      <c r="AL45" t="s">
+        <v>70</v>
+      </c>
+      <c r="AM45" s="1">
+        <v>43441</v>
+      </c>
+    </row>
+    <row r="46" spans="1:39">
+      <c r="A46" t="s">
+        <v>75</v>
+      </c>
+      <c r="C46" t="s">
+        <v>37</v>
+      </c>
+      <c r="D46" t="s">
+        <v>37</v>
+      </c>
+      <c r="E46" t="s">
+        <v>37</v>
+      </c>
+      <c r="I46" t="s">
+        <v>37</v>
+      </c>
+      <c r="K46" t="s">
+        <v>37</v>
+      </c>
+      <c r="N46" t="s">
+        <v>37</v>
+      </c>
+      <c r="O46" t="s">
+        <v>37</v>
+      </c>
+      <c r="P46" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q46" t="s">
+        <v>37</v>
+      </c>
+      <c r="V46" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK46">
+        <v>10</v>
+      </c>
+      <c r="AL46" t="s">
+        <v>44</v>
+      </c>
+      <c r="AM46" s="1">
+        <v>43441</v>
+      </c>
+    </row>
+    <row r="47" spans="1:39">
+      <c r="A47" t="s">
+        <v>71</v>
+      </c>
+      <c r="B47" t="s">
+        <v>37</v>
+      </c>
+      <c r="C47" t="s">
+        <v>37</v>
+      </c>
+      <c r="E47" t="s">
+        <v>37</v>
+      </c>
+      <c r="G47" t="s">
+        <v>37</v>
+      </c>
+      <c r="I47" t="s">
+        <v>37</v>
+      </c>
+      <c r="J47" t="s">
+        <v>37</v>
+      </c>
+      <c r="K47" t="s">
+        <v>37</v>
+      </c>
+      <c r="O47" t="s">
+        <v>37</v>
+      </c>
+      <c r="P47" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q47" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK47">
+        <v>10</v>
+      </c>
+      <c r="AL47" t="s">
+        <v>72</v>
+      </c>
+      <c r="AM47" s="1">
+        <v>43440</v>
+      </c>
+    </row>
+    <row r="48" spans="1:39">
+      <c r="A48" t="s">
+        <v>64</v>
+      </c>
+      <c r="C48" t="s">
+        <v>37</v>
+      </c>
+      <c r="D48" t="s">
+        <v>37</v>
+      </c>
+      <c r="E48" t="s">
+        <v>37</v>
+      </c>
+      <c r="I48" t="s">
+        <v>37</v>
+      </c>
+      <c r="K48" t="s">
+        <v>37</v>
+      </c>
+      <c r="M48" t="s">
+        <v>37</v>
+      </c>
+      <c r="N48" t="s">
+        <v>37</v>
+      </c>
+      <c r="O48" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q48" t="s">
+        <v>37</v>
+      </c>
+      <c r="V48" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK48">
+        <v>10</v>
+      </c>
+      <c r="AL48" t="s">
+        <v>65</v>
+      </c>
+      <c r="AM48" s="1">
+        <v>43439</v>
+      </c>
+    </row>
+    <row r="49" spans="1:39">
+      <c r="A49" t="s">
+        <v>69</v>
+      </c>
+      <c r="C49" t="s">
+        <v>37</v>
+      </c>
+      <c r="D49" t="s">
+        <v>37</v>
+      </c>
+      <c r="E49" t="s">
+        <v>37</v>
+      </c>
+      <c r="F49" t="s">
+        <v>37</v>
+      </c>
+      <c r="I49" t="s">
+        <v>37</v>
+      </c>
+      <c r="J49" t="s">
+        <v>37</v>
+      </c>
+      <c r="K49" t="s">
+        <v>37</v>
+      </c>
+      <c r="O49" t="s">
+        <v>37</v>
+      </c>
+      <c r="T49" t="s">
+        <v>37</v>
+      </c>
+      <c r="V49" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK49">
+        <v>10</v>
+      </c>
+      <c r="AL49" t="s">
+        <v>70</v>
+      </c>
+      <c r="AM49" s="1">
+        <v>43439</v>
+      </c>
+    </row>
+    <row r="50" spans="1:39">
+      <c r="A50" t="s">
+        <v>66</v>
+      </c>
+      <c r="E50" t="s">
+        <v>37</v>
+      </c>
+      <c r="I50" t="s">
+        <v>37</v>
+      </c>
+      <c r="J50" t="s">
+        <v>37</v>
+      </c>
+      <c r="K50" t="s">
+        <v>37</v>
+      </c>
+      <c r="M50" t="s">
+        <v>37</v>
+      </c>
+      <c r="O50" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q50" t="s">
+        <v>37</v>
+      </c>
+      <c r="T50" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK50">
+        <v>8</v>
+      </c>
+      <c r="AL50" t="s">
+        <v>67</v>
+      </c>
+      <c r="AM50" s="1">
+        <v>43439</v>
+      </c>
+    </row>
+    <row r="51" spans="1:39">
+      <c r="A51" t="s">
+        <v>68</v>
+      </c>
+      <c r="C51" t="s">
+        <v>37</v>
+      </c>
+      <c r="D51" t="s">
+        <v>37</v>
+      </c>
+      <c r="E51" t="s">
+        <v>37</v>
+      </c>
+      <c r="F51" t="s">
+        <v>37</v>
+      </c>
+      <c r="H51" t="s">
+        <v>37</v>
+      </c>
+      <c r="I51" t="s">
+        <v>37</v>
+      </c>
+      <c r="J51" t="s">
+        <v>37</v>
+      </c>
+      <c r="K51" t="s">
+        <v>37</v>
+      </c>
+      <c r="O51" t="s">
+        <v>37</v>
+      </c>
+      <c r="V51" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK51">
+        <v>10</v>
+      </c>
+      <c r="AL51" t="s">
+        <v>44</v>
+      </c>
+      <c r="AM51" s="1">
+        <v>43439</v>
+      </c>
+    </row>
+    <row r="52" spans="1:39">
+      <c r="A52" t="s">
+        <v>63</v>
+      </c>
+      <c r="C52" t="s">
+        <v>37</v>
+      </c>
+      <c r="D52" t="s">
+        <v>37</v>
+      </c>
+      <c r="E52" t="s">
+        <v>37</v>
+      </c>
+      <c r="I52" t="s">
+        <v>37</v>
+      </c>
+      <c r="K52" t="s">
+        <v>37</v>
+      </c>
+      <c r="M52" t="s">
+        <v>37</v>
+      </c>
+      <c r="O52" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q52" t="s">
+        <v>37</v>
+      </c>
+      <c r="T52" t="s">
+        <v>37</v>
+      </c>
+      <c r="V52" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK52">
+        <v>10</v>
+      </c>
+      <c r="AL52" t="s">
+        <v>42</v>
+      </c>
+      <c r="AM52" s="1">
+        <v>43437</v>
+      </c>
+    </row>
+    <row r="53" spans="1:39">
+      <c r="A53" t="s">
+        <v>62</v>
+      </c>
+      <c r="C53" t="s">
+        <v>37</v>
+      </c>
+      <c r="D53" t="s">
+        <v>37</v>
+      </c>
+      <c r="E53" t="s">
+        <v>37</v>
+      </c>
+      <c r="I53" t="s">
+        <v>37</v>
+      </c>
+      <c r="K53" t="s">
+        <v>37</v>
+      </c>
+      <c r="O53" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q53" t="s">
+        <v>37</v>
+      </c>
+      <c r="R53" t="s">
+        <v>37</v>
+      </c>
+      <c r="S53" t="s">
+        <v>37</v>
+      </c>
+      <c r="T53" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK53">
+        <v>10</v>
+      </c>
+      <c r="AL53" t="s">
+        <v>38</v>
+      </c>
+      <c r="AM53" s="1">
+        <v>43436</v>
+      </c>
+    </row>
+    <row r="54" spans="1:39">
+      <c r="A54" t="s">
+        <v>59</v>
+      </c>
+      <c r="C54" t="s">
+        <v>37</v>
+      </c>
+      <c r="D54" t="s">
+        <v>37</v>
+      </c>
+      <c r="E54" t="s">
+        <v>37</v>
+      </c>
+      <c r="I54" t="s">
+        <v>37</v>
+      </c>
+      <c r="K54" t="s">
+        <v>37</v>
+      </c>
+      <c r="O54" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q54" t="s">
+        <v>37</v>
+      </c>
+      <c r="S54" t="s">
+        <v>37</v>
+      </c>
+      <c r="T54" t="s">
+        <v>37</v>
+      </c>
+      <c r="V54" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK54">
+        <v>10</v>
+      </c>
+      <c r="AL54" t="s">
+        <v>60</v>
+      </c>
+      <c r="AM54" s="1">
+        <v>43434</v>
+      </c>
+    </row>
+    <row r="55" spans="1:39">
+      <c r="A55" t="s">
+        <v>61</v>
+      </c>
+      <c r="C55" t="s">
+        <v>37</v>
+      </c>
+      <c r="D55" t="s">
+        <v>37</v>
+      </c>
+      <c r="E55" t="s">
+        <v>37</v>
+      </c>
+      <c r="I55" t="s">
+        <v>37</v>
+      </c>
+      <c r="K55" t="s">
+        <v>37</v>
+      </c>
+      <c r="M55" t="s">
+        <v>37</v>
+      </c>
+      <c r="N55" t="s">
+        <v>37</v>
+      </c>
+      <c r="O55" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q55" t="s">
+        <v>37</v>
+      </c>
+      <c r="V55" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK55">
+        <v>10</v>
+      </c>
+      <c r="AL55" t="s">
+        <v>38</v>
+      </c>
+      <c r="AM55" s="1">
+        <v>43434</v>
+      </c>
+    </row>
+    <row r="56" spans="1:39">
+      <c r="A56" t="s">
+        <v>57</v>
+      </c>
+      <c r="C56" t="s">
+        <v>37</v>
+      </c>
+      <c r="D56" t="s">
+        <v>37</v>
+      </c>
+      <c r="E56" t="s">
+        <v>37</v>
+      </c>
+      <c r="I56" t="s">
+        <v>37</v>
+      </c>
+      <c r="K56" t="s">
+        <v>37</v>
+      </c>
+      <c r="O56" t="s">
+        <v>37</v>
+      </c>
+      <c r="S56" t="s">
+        <v>37</v>
+      </c>
+      <c r="T56" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK56">
+        <v>8</v>
+      </c>
+      <c r="AL56" t="s">
+        <v>58</v>
+      </c>
+      <c r="AM56" s="1">
+        <v>43433</v>
+      </c>
+    </row>
+    <row r="57" spans="1:39">
+      <c r="A57" t="s">
+        <v>54</v>
+      </c>
+      <c r="E57" t="s">
+        <v>37</v>
+      </c>
+      <c r="I57" t="s">
+        <v>37</v>
+      </c>
+      <c r="K57" t="s">
+        <v>37</v>
+      </c>
+      <c r="O57" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q57" t="s">
+        <v>37</v>
+      </c>
+      <c r="T57" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK57">
+        <v>6</v>
+      </c>
+      <c r="AL57" t="s">
+        <v>44</v>
+      </c>
+      <c r="AM57" s="1">
+        <v>43433</v>
+      </c>
+    </row>
+    <row r="58" spans="1:39">
+      <c r="A58" t="s">
+        <v>55</v>
+      </c>
+      <c r="C58" t="s">
+        <v>37</v>
+      </c>
+      <c r="D58" t="s">
+        <v>37</v>
+      </c>
+      <c r="E58" t="s">
+        <v>37</v>
+      </c>
+      <c r="I58" t="s">
+        <v>37</v>
+      </c>
+      <c r="N58" t="s">
+        <v>37</v>
+      </c>
+      <c r="O58" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK58">
+        <v>6</v>
+      </c>
+      <c r="AL58" t="s">
+        <v>56</v>
+      </c>
+      <c r="AM58" s="1">
+        <v>43433</v>
+      </c>
+    </row>
+    <row r="59" spans="1:39">
+      <c r="A59" t="s">
+        <v>39</v>
+      </c>
+      <c r="C59" t="s">
+        <v>37</v>
+      </c>
+      <c r="D59" t="s">
+        <v>37</v>
+      </c>
+      <c r="E59" t="s">
+        <v>37</v>
+      </c>
+      <c r="I59" t="s">
+        <v>37</v>
+      </c>
+      <c r="K59" t="s">
+        <v>37</v>
+      </c>
+      <c r="O59" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q59" t="s">
+        <v>37</v>
+      </c>
+      <c r="V59" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK59">
+        <v>8</v>
+      </c>
+      <c r="AL59" t="s">
+        <v>40</v>
+      </c>
+      <c r="AM59" s="1">
+        <v>43431</v>
+      </c>
+    </row>
+    <row r="60" spans="1:39">
+      <c r="A60" t="s">
+        <v>47</v>
+      </c>
+      <c r="C60" t="s">
+        <v>37</v>
+      </c>
+      <c r="D60" t="s">
+        <v>37</v>
+      </c>
+      <c r="I60" t="s">
+        <v>37</v>
+      </c>
+      <c r="K60" t="s">
+        <v>37</v>
+      </c>
+      <c r="M60" t="s">
+        <v>37</v>
+      </c>
+      <c r="N60" t="s">
+        <v>37</v>
+      </c>
+      <c r="O60" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q60" t="s">
+        <v>37</v>
+      </c>
+      <c r="T60" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK60">
+        <v>9</v>
+      </c>
+      <c r="AL60" t="s">
+        <v>46</v>
+      </c>
+      <c r="AM60" s="1">
+        <v>43430</v>
+      </c>
+    </row>
+    <row r="61" spans="1:39">
+      <c r="A61" t="s">
+        <v>43</v>
+      </c>
+      <c r="D61" t="s">
+        <v>37</v>
+      </c>
+      <c r="E61" t="s">
+        <v>37</v>
+      </c>
+      <c r="F61" t="s">
+        <v>37</v>
+      </c>
+      <c r="G61" t="s">
+        <v>37</v>
+      </c>
+      <c r="I61" t="s">
+        <v>37</v>
+      </c>
+      <c r="K61" t="s">
+        <v>37</v>
+      </c>
+      <c r="M61" t="s">
+        <v>37</v>
+      </c>
+      <c r="O61" t="s">
+        <v>37</v>
+      </c>
+      <c r="S61" t="s">
+        <v>37</v>
+      </c>
+      <c r="T61" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK61">
+        <v>10</v>
+      </c>
+      <c r="AL61" t="s">
+        <v>44</v>
+      </c>
+      <c r="AM61" s="1">
+        <v>43430</v>
+      </c>
+    </row>
+    <row r="62" spans="1:39">
+      <c r="A62" t="s">
+        <v>45</v>
+      </c>
+      <c r="I62" t="s">
+        <v>37</v>
+      </c>
+      <c r="O62" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK62">
+        <v>2</v>
+      </c>
+      <c r="AL62" t="s">
+        <v>46</v>
+      </c>
+      <c r="AM62" s="1">
+        <v>43430</v>
+      </c>
+    </row>
+    <row r="63" spans="1:39">
+      <c r="A63" t="s">
+        <v>36</v>
+      </c>
+      <c r="C63" t="s">
+        <v>37</v>
+      </c>
+      <c r="D63" t="s">
+        <v>37</v>
+      </c>
+      <c r="E63" t="s">
+        <v>37</v>
+      </c>
+      <c r="I63" t="s">
+        <v>37</v>
+      </c>
+      <c r="J63" t="s">
+        <v>37</v>
+      </c>
+      <c r="K63" t="s">
+        <v>37</v>
+      </c>
+      <c r="N63" t="s">
+        <v>37</v>
+      </c>
+      <c r="O63" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q63" t="s">
+        <v>37</v>
+      </c>
+      <c r="AH63" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK63">
+        <v>10</v>
+      </c>
+      <c r="AL63" t="s">
+        <v>38</v>
+      </c>
+      <c r="AM63" s="1">
+        <v>43429</v>
+      </c>
+    </row>
+    <row r="64" spans="1:39">
+      <c r="A64" t="s">
+        <v>41</v>
+      </c>
+      <c r="E64" t="s">
+        <v>37</v>
+      </c>
+      <c r="F64" t="s">
+        <v>37</v>
+      </c>
+      <c r="I64" t="s">
+        <v>37</v>
+      </c>
+      <c r="J64" t="s">
+        <v>37</v>
+      </c>
+      <c r="K64" t="s">
+        <v>37</v>
+      </c>
+      <c r="O64" t="s">
+        <v>37</v>
+      </c>
+      <c r="P64" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q64" t="s">
+        <v>37</v>
+      </c>
+      <c r="T64" t="s">
+        <v>37</v>
+      </c>
+      <c r="V64" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK64">
+        <v>10</v>
+      </c>
+      <c r="AL64" t="s">
+        <v>42</v>
+      </c>
+      <c r="AM64" s="1">
+        <v>43429</v>
+      </c>
+    </row>
+    <row r="65" spans="1:39">
+      <c r="A65" t="s">
+        <v>48</v>
+      </c>
+      <c r="C65" t="s">
+        <v>37</v>
+      </c>
+      <c r="D65" t="s">
+        <v>37</v>
+      </c>
+      <c r="E65" t="s">
+        <v>37</v>
+      </c>
+      <c r="F65" t="s">
+        <v>37</v>
+      </c>
+      <c r="I65" t="s">
+        <v>37</v>
+      </c>
+      <c r="O65" t="s">
+        <v>37</v>
+      </c>
+      <c r="P65" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q65" t="s">
+        <v>37</v>
+      </c>
+      <c r="T65" t="s">
+        <v>37</v>
+      </c>
+      <c r="V65" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK65">
+        <v>10</v>
+      </c>
+      <c r="AL65" t="s">
+        <v>44</v>
+      </c>
+      <c r="AM65" s="1">
+        <v>43426</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A1:AM65">
+    <sortCondition descending="1" ref="AM1:AM65"/>
+  </sortState>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>